<commit_message>
2022Q3 DCF Update for J.Jill (JILL)
Very underpriced (at the time of update Dec/7/2022).
Price target: $27.50
</commit_message>
<xml_diff>
--- a/DCF Models/JILL.xlsx
+++ b/DCF Models/JILL.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25330"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25726"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PC\Desktop\Fiduciary\Models\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PC\Desktop\Fiduciary\investingModels\DCF Models\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{073CDBB1-F7F7-4935-8C5D-2760DE5FACA0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9FC05395-C132-408D-8DE9-F7509651394B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="18930" yWindow="3480" windowWidth="32565" windowHeight="17250" activeTab="1" xr2:uid="{2EC0F4CB-CC56-4207-8108-7C832533A8D8}"/>
+    <workbookView xWindow="42555" yWindow="6720" windowWidth="44730" windowHeight="18825" activeTab="1" xr2:uid="{2EC0F4CB-CC56-4207-8108-7C832533A8D8}"/>
   </bookViews>
   <sheets>
     <sheet name="Main" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="47">
   <si>
     <t>Price</t>
   </si>
@@ -170,6 +170,12 @@
   <si>
     <t>Annual 10y Grow</t>
   </si>
+  <si>
+    <t>Target</t>
+  </si>
+  <si>
+    <t>SG&amp;A y/y</t>
+  </si>
 </sst>
 </file>
 
@@ -276,16 +282,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>65942</xdr:colOff>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>608867</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>65944</xdr:rowOff>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>65942</xdr:colOff>
-      <xdr:row>48</xdr:row>
-      <xdr:rowOff>43963</xdr:rowOff>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>608867</xdr:colOff>
+      <xdr:row>47</xdr:row>
+      <xdr:rowOff>168519</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
@@ -300,8 +306,8 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="8719038" y="65944"/>
-          <a:ext cx="0" cy="7979019"/>
+          <a:off x="8981342" y="0"/>
+          <a:ext cx="0" cy="9122019"/>
         </a:xfrm>
         <a:prstGeom prst="line">
           <a:avLst/>
@@ -727,7 +733,7 @@
   <dimension ref="M1:O20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="M11" sqref="M11"/>
+      <selection activeCell="U16" sqref="U16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -799,7 +805,7 @@
     </row>
     <row r="11" spans="13:15" x14ac:dyDescent="0.25">
       <c r="M11" s="19">
-        <v>44767</v>
+        <v>44902</v>
       </c>
     </row>
     <row r="16" spans="13:15" x14ac:dyDescent="0.25">
@@ -861,11 +867,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{430C4823-B1D5-4075-A061-9C811CDAD08D}">
   <dimension ref="B1:HH31"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <pane xSplit="2" ySplit="2" topLeftCell="Q3" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="2" ySplit="2" topLeftCell="S3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="Z15" sqref="Z15"/>
+      <selection pane="bottomRight" activeCell="X35" sqref="X35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -876,6 +882,7 @@
     <col min="13" max="13" width="9.140625" style="5"/>
     <col min="16" max="16" width="4.42578125" style="11" customWidth="1"/>
     <col min="35" max="35" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="10" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:216" x14ac:dyDescent="0.25">
@@ -1010,6 +1017,12 @@
       <c r="K3" s="5">
         <v>157.06899999999999</v>
       </c>
+      <c r="L3" s="5">
+        <v>160.34</v>
+      </c>
+      <c r="M3" s="5">
+        <v>150.19999999999999</v>
+      </c>
       <c r="N3" s="5"/>
       <c r="Q3" s="1">
         <v>698.1</v>
@@ -1033,48 +1046,48 @@
         <v>628.27599999999995</v>
       </c>
       <c r="W3" s="5">
-        <f>V3*1.07</f>
-        <v>672.25531999999998</v>
+        <f>V3*(1+W28)</f>
+        <v>578.01391999999998</v>
       </c>
       <c r="X3" s="5">
-        <f>W3*1.07</f>
-        <v>719.31319240000005</v>
+        <f>W3*(1+X28)</f>
+        <v>635.81531200000006</v>
       </c>
       <c r="Y3" s="5">
-        <f>X3*1.07</f>
-        <v>769.66511586800004</v>
+        <f t="shared" ref="Y3:AG3" si="0">X3*(1+Y28)</f>
+        <v>667.60607760000005</v>
       </c>
       <c r="Z3" s="5">
-        <f>Y3*1.07</f>
-        <v>823.54167397876006</v>
+        <f t="shared" si="0"/>
+        <v>714.33850303200006</v>
       </c>
       <c r="AA3" s="5">
-        <f>Z3*1.05</f>
-        <v>864.71875767769814</v>
+        <f t="shared" si="0"/>
+        <v>764.34219824424008</v>
       </c>
       <c r="AB3" s="5">
-        <f>AA3*1.05</f>
-        <v>907.95469556158309</v>
+        <f t="shared" si="0"/>
+        <v>802.55930815645206</v>
       </c>
       <c r="AC3" s="5">
-        <f>AB3*1.05</f>
-        <v>953.35243033966231</v>
+        <f t="shared" si="0"/>
+        <v>842.68727356427473</v>
       </c>
       <c r="AD3" s="5">
-        <f>AC3*1.03</f>
-        <v>981.95300324985215</v>
+        <f t="shared" si="0"/>
+        <v>867.96789177120297</v>
       </c>
       <c r="AE3" s="5">
-        <f>AD3*1.03</f>
-        <v>1011.4115933473478</v>
+        <f t="shared" si="0"/>
+        <v>894.00692852433906</v>
       </c>
       <c r="AF3" s="5">
-        <f>AE3*1.03</f>
-        <v>1041.7539411477683</v>
+        <f t="shared" si="0"/>
+        <v>920.82713638006931</v>
       </c>
       <c r="AG3" s="5">
-        <f>AF3*1.01</f>
-        <v>1052.171480559246</v>
+        <f t="shared" si="0"/>
+        <v>930.03540774387</v>
       </c>
       <c r="AH3" s="1"/>
       <c r="AI3" s="1"/>
@@ -1154,6 +1167,12 @@
       <c r="K4" s="5">
         <v>47.6</v>
       </c>
+      <c r="L4" s="5">
+        <v>47.87</v>
+      </c>
+      <c r="M4" s="5">
+        <v>45.18</v>
+      </c>
       <c r="N4" s="5"/>
       <c r="Q4" s="1">
         <v>198.5</v>
@@ -1165,11 +1184,11 @@
         <v>262.76</v>
       </c>
       <c r="T4" s="1">
-        <f t="shared" ref="T4:T15" si="0">SUM(C4:F4)</f>
+        <f t="shared" ref="T4:T13" si="1">SUM(C4:F4)</f>
         <v>181.136</v>
       </c>
       <c r="U4" s="5">
-        <f t="shared" ref="U4:U13" si="1">SUM(G4:J4)</f>
+        <f t="shared" ref="U4:U13" si="2">SUM(G4:J4)</f>
         <v>190.77</v>
       </c>
       <c r="V4" s="5"/>
@@ -1236,43 +1255,49 @@
         <v>17</v>
       </c>
       <c r="C5" s="4">
-        <f t="shared" ref="C5" si="2">C3-C4</f>
+        <f t="shared" ref="C5" si="3">C3-C4</f>
         <v>50.168999999999997</v>
       </c>
       <c r="D5" s="4">
-        <f t="shared" ref="C5:K5" si="3">D3-D4</f>
+        <f t="shared" ref="D5:K5" si="4">D3-D4</f>
         <v>55.019999999999996</v>
       </c>
       <c r="E5" s="4">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>69</v>
       </c>
       <c r="F5" s="4">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>71.400000000000006</v>
       </c>
       <c r="G5" s="4">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>87.84</v>
       </c>
       <c r="H5" s="4">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>109.35</v>
       </c>
       <c r="I5" s="4">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>104.52999999999999</v>
       </c>
       <c r="J5" s="4">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>92.72</v>
       </c>
       <c r="K5" s="4">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>109.46899999999999</v>
       </c>
-      <c r="L5" s="4"/>
-      <c r="M5" s="4"/>
+      <c r="L5" s="4">
+        <f t="shared" ref="L5:M5" si="5">L3-L4</f>
+        <v>112.47</v>
+      </c>
+      <c r="M5" s="4">
+        <f t="shared" si="5"/>
+        <v>105.01999999999998</v>
+      </c>
       <c r="N5" s="4"/>
       <c r="P5" s="12"/>
       <c r="Q5" s="4">
@@ -1288,60 +1313,60 @@
         <v>428.53999999999996</v>
       </c>
       <c r="T5" s="4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>245.589</v>
       </c>
       <c r="U5" s="4">
-        <f t="shared" si="1"/>
+        <f>SUM(G5:J5)</f>
         <v>394.43999999999994</v>
       </c>
       <c r="V5" s="4">
-        <f>V3*0.66</f>
-        <v>414.66215999999997</v>
+        <f>V3*V23</f>
+        <v>439.79319999999996</v>
       </c>
       <c r="W5" s="4">
-        <f>W3*0.66</f>
-        <v>443.68851119999999</v>
+        <f>W3*W23</f>
+        <v>404.60974399999998</v>
       </c>
       <c r="X5" s="4">
-        <f>X3*0.66</f>
-        <v>474.74670698400007</v>
+        <f t="shared" ref="X5:AG5" si="6">X3*X23</f>
+        <v>445.07071840000003</v>
       </c>
       <c r="Y5" s="4">
-        <f>Y3*0.66</f>
-        <v>507.97897647288005</v>
+        <f t="shared" si="6"/>
+        <v>467.32425432000002</v>
       </c>
       <c r="Z5" s="4">
-        <f>Z3*0.66</f>
-        <v>543.53750482598161</v>
+        <f t="shared" si="6"/>
+        <v>500.03695212240001</v>
       </c>
       <c r="AA5" s="4">
-        <f>AA3*0.66</f>
-        <v>570.71438006728079</v>
+        <f t="shared" si="6"/>
+        <v>535.03953877096808</v>
       </c>
       <c r="AB5" s="4">
-        <f>AB3*0.66</f>
-        <v>599.25009907064486</v>
+        <f t="shared" si="6"/>
+        <v>561.79151570951637</v>
       </c>
       <c r="AC5" s="4">
-        <f>AC3*0.66</f>
-        <v>629.21260402417715</v>
+        <f t="shared" si="6"/>
+        <v>589.88109149499223</v>
       </c>
       <c r="AD5" s="4">
-        <f>AD3*0.66</f>
-        <v>648.0889821449025</v>
+        <f t="shared" si="6"/>
+        <v>607.57752423984209</v>
       </c>
       <c r="AE5" s="4">
-        <f>AE3*0.66</f>
-        <v>667.53165160924959</v>
+        <f t="shared" si="6"/>
+        <v>625.80484996703728</v>
       </c>
       <c r="AF5" s="4">
-        <f>AF3*0.66</f>
-        <v>687.55760115752707</v>
+        <f t="shared" si="6"/>
+        <v>644.57899546604847</v>
       </c>
       <c r="AG5" s="4">
-        <f>AG3*0.66</f>
-        <v>694.43317716910235</v>
+        <f t="shared" si="6"/>
+        <v>651.02478542070901</v>
       </c>
       <c r="AH5" s="4"/>
       <c r="AI5" s="4"/>
@@ -1421,6 +1446,12 @@
       <c r="K6" s="5">
         <v>85.6</v>
       </c>
+      <c r="L6" s="5">
+        <v>84.281000000000006</v>
+      </c>
+      <c r="M6" s="5">
+        <v>84.87</v>
+      </c>
       <c r="N6" s="5"/>
       <c r="Q6" s="1">
         <v>402</v>
@@ -1432,11 +1463,11 @@
         <v>380</v>
       </c>
       <c r="T6" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>343.20000000000005</v>
       </c>
       <c r="U6" s="5">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>335.68</v>
       </c>
       <c r="V6" s="5">
@@ -1448,43 +1479,43 @@
         <v>370.0872</v>
       </c>
       <c r="X6" s="5">
-        <f>W6*1.05</f>
+        <f t="shared" ref="X6:AG6" si="7">W6*1.05</f>
         <v>388.59156000000002</v>
       </c>
       <c r="Y6" s="5">
-        <f>X6*1.05</f>
+        <f t="shared" si="7"/>
         <v>408.02113800000001</v>
       </c>
       <c r="Z6" s="5">
-        <f>Y6*1.05</f>
+        <f t="shared" si="7"/>
         <v>428.42219490000002</v>
       </c>
       <c r="AA6" s="5">
-        <f>Z6*1.05</f>
+        <f t="shared" si="7"/>
         <v>449.84330464500005</v>
       </c>
       <c r="AB6" s="5">
-        <f>AA6*1.05</f>
+        <f t="shared" si="7"/>
         <v>472.33546987725009</v>
       </c>
       <c r="AC6" s="5">
-        <f>AB6*1.05</f>
+        <f t="shared" si="7"/>
         <v>495.95224337111262</v>
       </c>
       <c r="AD6" s="5">
-        <f>AC6*1.05</f>
+        <f t="shared" si="7"/>
         <v>520.74985553966826</v>
       </c>
       <c r="AE6" s="5">
-        <f>AD6*1.05</f>
+        <f t="shared" si="7"/>
         <v>546.78734831665167</v>
       </c>
       <c r="AF6" s="5">
-        <f>AE6*1.05</f>
+        <f t="shared" si="7"/>
         <v>574.12671573248429</v>
       </c>
       <c r="AG6" s="5">
-        <f>AF6*1.05</f>
+        <f t="shared" si="7"/>
         <v>602.83305151910849</v>
       </c>
       <c r="AH6" s="1"/>
@@ -1567,16 +1598,22 @@
       <c r="K7" s="5">
         <v>0</v>
       </c>
+      <c r="L7" s="5">
+        <v>0</v>
+      </c>
+      <c r="M7" s="5">
+        <v>1.3</v>
+      </c>
       <c r="N7" s="5"/>
       <c r="Q7" s="1"/>
       <c r="R7" s="1"/>
       <c r="S7" s="1"/>
       <c r="T7" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>66.296999999999997</v>
       </c>
       <c r="U7" s="5">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="V7" s="5"/>
@@ -1643,51 +1680,59 @@
         <v>21</v>
       </c>
       <c r="C8" s="5">
-        <f t="shared" ref="C8" si="4">+C6+C4+C7</f>
+        <f t="shared" ref="C8" si="8">+C6+C4+C7</f>
         <v>180.7</v>
       </c>
       <c r="D8" s="5">
-        <f t="shared" ref="D8:K8" si="5">+D6+D4+D7</f>
+        <f t="shared" ref="D8:K8" si="9">+D6+D4+D7</f>
         <v>114.423</v>
       </c>
       <c r="E8" s="5">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>141.126</v>
       </c>
       <c r="F8" s="5">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>154.38399999999999</v>
       </c>
       <c r="G8" s="5">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>120.35999999999999</v>
       </c>
       <c r="H8" s="5">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>135.72999999999999</v>
       </c>
       <c r="I8" s="5">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>132.73000000000002</v>
       </c>
       <c r="J8" s="5">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>137.63</v>
       </c>
       <c r="K8" s="5">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>133.19999999999999</v>
+      </c>
+      <c r="L8" s="5">
+        <f t="shared" ref="L8:M8" si="10">+L6+L4+L7</f>
+        <v>132.15100000000001</v>
+      </c>
+      <c r="M8" s="5">
+        <f t="shared" si="10"/>
+        <v>131.35000000000002</v>
       </c>
       <c r="N8" s="5"/>
       <c r="Q8" s="1"/>
       <c r="R8" s="1"/>
       <c r="S8" s="1"/>
       <c r="T8" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>590.63300000000004</v>
       </c>
       <c r="U8" s="5">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>526.45000000000005</v>
       </c>
       <c r="V8" s="5"/>
@@ -1754,43 +1799,49 @@
         <v>22</v>
       </c>
       <c r="C9" s="4">
-        <f t="shared" ref="C9" si="6">+C3-C8</f>
+        <f t="shared" ref="C9" si="11">+C3-C8</f>
         <v>-89.730999999999995</v>
       </c>
       <c r="D9" s="4">
-        <f t="shared" ref="D9:K9" si="7">+D3-D8</f>
+        <f t="shared" ref="D9:K9" si="12">+D3-D8</f>
         <v>-21.787000000000006</v>
       </c>
       <c r="E9" s="4">
-        <f t="shared" si="7"/>
+        <f t="shared" si="12"/>
         <v>-23.906000000000006</v>
       </c>
       <c r="F9" s="4">
-        <f t="shared" si="7"/>
+        <f t="shared" si="12"/>
         <v>-28.48399999999998</v>
       </c>
       <c r="G9" s="4">
-        <f t="shared" si="7"/>
+        <f t="shared" si="12"/>
         <v>8.7400000000000091</v>
       </c>
       <c r="H9" s="4">
-        <f t="shared" si="7"/>
+        <f t="shared" si="12"/>
         <v>23.5</v>
       </c>
       <c r="I9" s="4">
-        <f t="shared" si="7"/>
+        <f t="shared" si="12"/>
         <v>18.999999999999972</v>
       </c>
       <c r="J9" s="4">
-        <f t="shared" si="7"/>
+        <f t="shared" si="12"/>
         <v>7.5200000000000102</v>
       </c>
       <c r="K9" s="4">
-        <f t="shared" si="7"/>
+        <f t="shared" si="12"/>
         <v>23.869</v>
       </c>
-      <c r="L9" s="4"/>
-      <c r="M9" s="4"/>
+      <c r="L9" s="4">
+        <f t="shared" ref="L9:M9" si="13">+L3-L8</f>
+        <v>28.188999999999993</v>
+      </c>
+      <c r="M9" s="4">
+        <f t="shared" si="13"/>
+        <v>18.849999999999966</v>
+      </c>
       <c r="N9" s="4"/>
       <c r="P9" s="12"/>
       <c r="Q9" s="4">
@@ -1806,60 +1857,60 @@
         <v>48.539999999999964</v>
       </c>
       <c r="T9" s="4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>-163.90799999999999</v>
       </c>
       <c r="U9" s="4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>58.759999999999991</v>
       </c>
       <c r="V9" s="4">
-        <f>V5-V6</f>
-        <v>62.198159999999973</v>
+        <f t="shared" ref="V9:AG9" si="14">V5-V6</f>
+        <v>87.329199999999958</v>
       </c>
       <c r="W9" s="4">
-        <f>W5-W6</f>
-        <v>73.601311199999998</v>
+        <f t="shared" si="14"/>
+        <v>34.522543999999982</v>
       </c>
       <c r="X9" s="4">
-        <f>X5-X6</f>
-        <v>86.155146984000055</v>
+        <f t="shared" si="14"/>
+        <v>56.479158400000017</v>
       </c>
       <c r="Y9" s="4">
-        <f>Y5-Y6</f>
-        <v>99.957838472880042</v>
+        <f t="shared" si="14"/>
+        <v>59.303116320000015</v>
       </c>
       <c r="Z9" s="4">
-        <f>Z5-Z6</f>
-        <v>115.11530992598159</v>
+        <f t="shared" si="14"/>
+        <v>71.614757222399987</v>
       </c>
       <c r="AA9" s="4">
-        <f>AA5-AA6</f>
-        <v>120.87107542228074</v>
+        <f t="shared" si="14"/>
+        <v>85.196234125968033</v>
       </c>
       <c r="AB9" s="4">
-        <f>AB5-AB6</f>
-        <v>126.91462919339477</v>
+        <f t="shared" si="14"/>
+        <v>89.456045832266284</v>
       </c>
       <c r="AC9" s="4">
-        <f>AC5-AC6</f>
-        <v>133.26036065306454</v>
+        <f t="shared" si="14"/>
+        <v>93.928848123879618</v>
       </c>
       <c r="AD9" s="4">
-        <f>AD5-AD6</f>
-        <v>127.33912660523424</v>
+        <f t="shared" si="14"/>
+        <v>86.827668700173831</v>
       </c>
       <c r="AE9" s="4">
-        <f>AE5-AE6</f>
-        <v>120.74430329259792</v>
+        <f t="shared" si="14"/>
+        <v>79.017501650385611</v>
       </c>
       <c r="AF9" s="4">
-        <f>AF5-AF6</f>
-        <v>113.43088542504279</v>
+        <f t="shared" si="14"/>
+        <v>70.452279733564183</v>
       </c>
       <c r="AG9" s="4">
-        <f>AG5-AG6</f>
-        <v>91.600125649993856</v>
+        <f t="shared" si="14"/>
+        <v>48.191733901600514</v>
       </c>
       <c r="AH9" s="4"/>
       <c r="AI9" s="4"/>
@@ -1942,16 +1993,22 @@
       <c r="K10" s="5">
         <v>0</v>
       </c>
+      <c r="L10" s="5">
+        <v>0</v>
+      </c>
+      <c r="M10" s="5">
+        <v>0</v>
+      </c>
       <c r="N10" s="5"/>
       <c r="Q10" s="1"/>
       <c r="R10" s="1"/>
       <c r="S10" s="1"/>
       <c r="T10" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>5.1899999999999995</v>
       </c>
       <c r="U10" s="5">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>59.754999999999995</v>
       </c>
       <c r="V10" s="5"/>
@@ -2050,8 +2107,14 @@
         <f>3.65+0.8</f>
         <v>4.45</v>
       </c>
-      <c r="L11" s="4"/>
-      <c r="M11" s="4"/>
+      <c r="L11" s="5">
+        <f>3.547+0.929</f>
+        <v>4.476</v>
+      </c>
+      <c r="M11" s="5">
+        <f>4.348+1.092</f>
+        <v>5.4399999999999995</v>
+      </c>
       <c r="N11" s="4"/>
       <c r="P11" s="12"/>
       <c r="Q11" s="5">
@@ -2064,11 +2127,11 @@
         <v>19.600000000000001</v>
       </c>
       <c r="T11" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>18.225000000000001</v>
       </c>
       <c r="U11" s="5">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>19.079000000000001</v>
       </c>
       <c r="V11" s="5">
@@ -2077,47 +2140,47 @@
       </c>
       <c r="W11" s="5">
         <f>W19*-0.105</f>
-        <v>18.08069004</v>
+        <v>16.431465540000001</v>
       </c>
       <c r="X11" s="5">
         <f>X19*-0.105</f>
-        <v>13.521587373000001</v>
+        <v>16.595411996100005</v>
       </c>
       <c r="Y11" s="5">
         <f>Y19*-0.105</f>
-        <v>7.2545655474809951</v>
+        <v>14.744239895290505</v>
       </c>
       <c r="Z11" s="5">
         <f>Z19*-0.015</f>
-        <v>-0.14637300581362653</v>
+        <v>1.7884300294108582</v>
       </c>
       <c r="AA11" s="5">
         <f>AA19*-0.015</f>
-        <v>-1.6529419978162896</v>
+        <v>1.1160628356078215</v>
       </c>
       <c r="AB11" s="5">
         <f>AB19*-0.015</f>
-        <v>-3.2573281945447659</v>
+        <v>0.25613992033064442</v>
       </c>
       <c r="AC11" s="5">
         <f>AC19*-0.01</f>
-        <v>-3.3098398583748212</v>
+        <v>-0.44034335437750188</v>
       </c>
       <c r="AD11" s="5">
-        <f t="shared" ref="AD11:AG11" si="8">AD19*-0.01</f>
-        <v>-4.5039384260280757</v>
+        <f t="shared" ref="AD11:AG11" si="15">AD19*-0.01</f>
+        <v>-1.089094723412577</v>
       </c>
       <c r="AE11" s="5">
-        <f t="shared" si="8"/>
-        <v>-5.6456175357557257</v>
+        <f t="shared" si="15"/>
+        <v>-1.6644735955285199</v>
       </c>
       <c r="AF11" s="5">
-        <f t="shared" si="8"/>
-        <v>-6.7274626572367389</v>
+        <f t="shared" si="15"/>
+        <v>-2.1583909230041427</v>
       </c>
       <c r="AG11" s="5">
-        <f t="shared" si="8"/>
-        <v>-7.7415304286529363</v>
+        <f t="shared" si="15"/>
+        <v>-2.5622081318368015</v>
       </c>
       <c r="AH11" s="4"/>
       <c r="AI11" s="4"/>
@@ -2197,8 +2260,12 @@
       <c r="K12" s="5">
         <v>5.01</v>
       </c>
-      <c r="L12" s="4"/>
-      <c r="M12" s="4"/>
+      <c r="L12" s="5">
+        <v>5.9119999999999999</v>
+      </c>
+      <c r="M12" s="5">
+        <v>4.49</v>
+      </c>
       <c r="N12" s="4"/>
       <c r="P12" s="12"/>
       <c r="Q12" s="5">
@@ -2211,60 +2278,60 @@
         <v>-3</v>
       </c>
       <c r="T12" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>-48.112000000000002</v>
       </c>
       <c r="U12" s="5">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>8.0139999999999993</v>
       </c>
       <c r="V12" s="5">
-        <f>V3*0.018</f>
-        <v>11.308967999999998</v>
+        <f>V3*V25</f>
+        <v>20.733107999999998</v>
       </c>
       <c r="W12" s="5">
-        <f t="shared" ref="W12:AG12" si="9">W3*0.018</f>
-        <v>12.100595759999999</v>
+        <f t="shared" ref="W12:AG12" si="16">W3*W25</f>
+        <v>19.652473280000002</v>
       </c>
       <c r="X12" s="5">
-        <f t="shared" si="9"/>
-        <v>12.9476374632</v>
+        <f t="shared" si="16"/>
+        <v>22.253535920000004</v>
       </c>
       <c r="Y12" s="5">
-        <f t="shared" si="9"/>
-        <v>13.853972085623999</v>
+        <f t="shared" si="16"/>
+        <v>23.366212716000003</v>
       </c>
       <c r="Z12" s="5">
-        <f t="shared" si="9"/>
-        <v>14.823750131617681</v>
+        <f t="shared" si="16"/>
+        <v>25.001847606120005</v>
       </c>
       <c r="AA12" s="5">
-        <f t="shared" si="9"/>
-        <v>15.564937638198565</v>
+        <f t="shared" si="16"/>
+        <v>26.751976938548406</v>
       </c>
       <c r="AB12" s="5">
-        <f t="shared" si="9"/>
-        <v>16.343184520108494</v>
+        <f t="shared" si="16"/>
+        <v>28.089575785475827</v>
       </c>
       <c r="AC12" s="5">
-        <f t="shared" si="9"/>
-        <v>17.16034374611392</v>
+        <f t="shared" si="16"/>
+        <v>29.494054574749619</v>
       </c>
       <c r="AD12" s="5">
-        <f t="shared" si="9"/>
-        <v>17.675154058497338</v>
+        <f t="shared" si="16"/>
+        <v>30.378876211992107</v>
       </c>
       <c r="AE12" s="5">
-        <f t="shared" si="9"/>
-        <v>18.205408680252258</v>
+        <f t="shared" si="16"/>
+        <v>31.290242498351869</v>
       </c>
       <c r="AF12" s="5">
-        <f t="shared" si="9"/>
-        <v>18.751570940659828</v>
+        <f t="shared" si="16"/>
+        <v>32.228949773302432</v>
       </c>
       <c r="AG12" s="5">
-        <f t="shared" si="9"/>
-        <v>18.939086650066425</v>
+        <f t="shared" si="16"/>
+        <v>32.551239271035456</v>
       </c>
       <c r="AH12" s="4"/>
       <c r="AI12" s="4"/>
@@ -2318,43 +2385,49 @@
         <v>20</v>
       </c>
       <c r="C13" s="4">
-        <f t="shared" ref="C13" si="10">+C9-C12-C11-C10</f>
+        <f t="shared" ref="C13" si="17">+C9-C12-C11-C10</f>
         <v>-70.271000000000001</v>
       </c>
       <c r="D13" s="4">
-        <f t="shared" ref="D13:K13" si="11">+D9-D12-D11-D10</f>
+        <f t="shared" ref="D13:K13" si="18">+D9-D12-D11-D10</f>
         <v>-19.031000000000006</v>
       </c>
       <c r="E13" s="4">
-        <f t="shared" si="11"/>
+        <f t="shared" si="18"/>
         <v>-22.946000000000009</v>
       </c>
       <c r="F13" s="4">
-        <f t="shared" si="11"/>
+        <f t="shared" si="18"/>
         <v>-26.962999999999983</v>
       </c>
       <c r="G13" s="4">
-        <f t="shared" si="11"/>
+        <f t="shared" si="18"/>
         <v>-18.258999999999986</v>
       </c>
       <c r="H13" s="4">
-        <f t="shared" si="11"/>
+        <f t="shared" si="18"/>
         <v>-24.644999999999996</v>
       </c>
       <c r="I13" s="4">
-        <f t="shared" si="11"/>
+        <f t="shared" si="18"/>
         <v>11.242999999999972</v>
       </c>
       <c r="J13" s="4">
-        <f t="shared" si="11"/>
+        <f t="shared" si="18"/>
         <v>3.5730000000000102</v>
       </c>
       <c r="K13" s="4">
-        <f t="shared" si="11"/>
+        <f t="shared" si="18"/>
         <v>14.409000000000002</v>
       </c>
-      <c r="L13" s="4"/>
-      <c r="M13" s="4"/>
+      <c r="L13" s="4">
+        <f t="shared" ref="L13:M13" si="19">+L9-L12-L11-L10</f>
+        <v>17.800999999999995</v>
+      </c>
+      <c r="M13" s="4">
+        <f t="shared" si="19"/>
+        <v>8.9199999999999662</v>
+      </c>
       <c r="N13" s="4"/>
       <c r="P13" s="12"/>
       <c r="Q13" s="4">
@@ -2367,792 +2440,792 @@
         <v>-128.6</v>
       </c>
       <c r="T13" s="4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>-139.21100000000001</v>
       </c>
       <c r="U13" s="4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>-28.087999999999997</v>
       </c>
       <c r="V13" s="4">
-        <f>V9-V11-V12</f>
-        <v>29.690951999999974</v>
+        <f t="shared" ref="V13:AG13" si="20">V9-V11-V12</f>
+        <v>45.397851999999958</v>
       </c>
       <c r="W13" s="4">
-        <f>W9-W11-W12</f>
-        <v>43.4200254</v>
+        <f t="shared" si="20"/>
+        <v>-1.5613948200000216</v>
       </c>
       <c r="X13" s="4">
-        <f>X9-X11-X12</f>
-        <v>59.685922147800056</v>
+        <f t="shared" si="20"/>
+        <v>17.630210483900008</v>
       </c>
       <c r="Y13" s="4">
-        <f>Y9-Y11-Y12</f>
-        <v>78.849300839775054</v>
+        <f t="shared" si="20"/>
+        <v>21.192663708709507</v>
       </c>
       <c r="Z13" s="4">
-        <f>Z9-Z11-Z12</f>
-        <v>100.43793280017753</v>
+        <f t="shared" si="20"/>
+        <v>44.824479586869117</v>
       </c>
       <c r="AA13" s="4">
-        <f>AA9-AA11-AA12</f>
-        <v>106.95907978189845</v>
+        <f t="shared" si="20"/>
+        <v>57.328194351811803</v>
       </c>
       <c r="AB13" s="4">
-        <f>AB9-AB11-AB12</f>
-        <v>113.82877286783103</v>
+        <f t="shared" si="20"/>
+        <v>61.110330126459814</v>
       </c>
       <c r="AC13" s="4">
-        <f>AC9-AC11-AC12</f>
-        <v>119.40985676532544</v>
+        <f t="shared" si="20"/>
+        <v>64.875136903507496</v>
       </c>
       <c r="AD13" s="4">
-        <f>AD9-AD11-AD12</f>
-        <v>114.16791097276497</v>
+        <f t="shared" si="20"/>
+        <v>57.537887211594295</v>
       </c>
       <c r="AE13" s="4">
-        <f>AE9-AE11-AE12</f>
-        <v>108.18451214810138</v>
+        <f t="shared" si="20"/>
+        <v>49.391732747562259</v>
       </c>
       <c r="AF13" s="4">
-        <f>AF9-AF11-AF12</f>
-        <v>101.4067771416197</v>
+        <f t="shared" si="20"/>
+        <v>40.381720883265899</v>
       </c>
       <c r="AG13" s="4">
-        <f>AG9-AG11-AG12</f>
-        <v>80.402569428580364</v>
+        <f t="shared" si="20"/>
+        <v>18.202702762401863</v>
       </c>
       <c r="AH13" s="4">
-        <f>AG13*(1+$AK21)</f>
-        <v>79.598543734294566</v>
+        <f t="shared" ref="AH13:BM13" si="21">AG13*(1+$AK21)</f>
+        <v>18.020675734777843</v>
       </c>
       <c r="AI13" s="4">
-        <f>AH13*(1+$AK21)</f>
-        <v>78.802558296951617</v>
+        <f t="shared" si="21"/>
+        <v>17.840468977430064</v>
       </c>
       <c r="AJ13" s="4">
-        <f>AI13*(1+$AK21)</f>
-        <v>78.014532713982106</v>
+        <f t="shared" si="21"/>
+        <v>17.662064287655763</v>
       </c>
       <c r="AK13" s="4">
-        <f>AJ13*(1+$AK21)</f>
-        <v>77.234387386842286</v>
+        <f t="shared" si="21"/>
+        <v>17.485443644779206</v>
       </c>
       <c r="AL13" s="4">
-        <f>AK13*(1+$AK21)</f>
-        <v>76.462043512973864</v>
+        <f t="shared" si="21"/>
+        <v>17.310589208331415</v>
       </c>
       <c r="AM13" s="4">
-        <f>AL13*(1+$AK21)</f>
-        <v>75.697423077844121</v>
+        <f t="shared" si="21"/>
+        <v>17.137483316248101</v>
       </c>
       <c r="AN13" s="4">
-        <f>AM13*(1+$AK21)</f>
-        <v>74.940448847065682</v>
+        <f t="shared" si="21"/>
+        <v>16.96610848308562</v>
       </c>
       <c r="AO13" s="4">
-        <f>AN13*(1+$AK21)</f>
-        <v>74.191044358595022</v>
+        <f t="shared" si="21"/>
+        <v>16.796447398254763</v>
       </c>
       <c r="AP13" s="4">
-        <f>AO13*(1+$AK21)</f>
-        <v>73.449133915009071</v>
+        <f t="shared" si="21"/>
+        <v>16.628482924272216</v>
       </c>
       <c r="AQ13" s="4">
-        <f>AP13*(1+$AK21)</f>
-        <v>72.714642575858974</v>
+        <f t="shared" si="21"/>
+        <v>16.462198095029493</v>
       </c>
       <c r="AR13" s="4">
-        <f>AQ13*(1+$AK21)</f>
-        <v>71.987496150100384</v>
+        <f t="shared" si="21"/>
+        <v>16.297576114079199</v>
       </c>
       <c r="AS13" s="4">
-        <f>AR13*(1+$AK21)</f>
-        <v>71.267621188599378</v>
+        <f t="shared" si="21"/>
+        <v>16.134600352938406</v>
       </c>
       <c r="AT13" s="4">
-        <f>AS13*(1+$AK21)</f>
-        <v>70.554944976713386</v>
+        <f t="shared" si="21"/>
+        <v>15.973254349409022</v>
       </c>
       <c r="AU13" s="4">
-        <f>AT13*(1+$AK21)</f>
-        <v>69.849395526946253</v>
+        <f t="shared" si="21"/>
+        <v>15.813521805914931</v>
       </c>
       <c r="AV13" s="4">
-        <f>AU13*(1+$AK21)</f>
-        <v>69.150901571676783</v>
+        <f t="shared" si="21"/>
+        <v>15.655386587855782</v>
       </c>
       <c r="AW13" s="4">
-        <f>AV13*(1+$AK21)</f>
-        <v>68.459392555960008</v>
+        <f t="shared" si="21"/>
+        <v>15.498832721977223</v>
       </c>
       <c r="AX13" s="4">
-        <f>AW13*(1+$AK21)</f>
-        <v>67.774798630400412</v>
+        <f t="shared" si="21"/>
+        <v>15.343844394757451</v>
       </c>
       <c r="AY13" s="4">
-        <f>AX13*(1+$AK21)</f>
-        <v>67.097050644096413</v>
+        <f t="shared" si="21"/>
+        <v>15.190405950809875</v>
       </c>
       <c r="AZ13" s="4">
-        <f>AY13*(1+$AK21)</f>
-        <v>66.426080137655447</v>
+        <f t="shared" si="21"/>
+        <v>15.038501891301777</v>
       </c>
       <c r="BA13" s="4">
-        <f>AZ13*(1+$AK21)</f>
-        <v>65.76181933627889</v>
+        <f t="shared" si="21"/>
+        <v>14.888116872388759</v>
       </c>
       <c r="BB13" s="4">
-        <f>BA13*(1+$AK21)</f>
-        <v>65.104201142916097</v>
+        <f t="shared" si="21"/>
+        <v>14.739235703664871</v>
       </c>
       <c r="BC13" s="4">
-        <f>BB13*(1+$AK21)</f>
-        <v>64.453159131486942</v>
+        <f t="shared" si="21"/>
+        <v>14.591843346628222</v>
       </c>
       <c r="BD13" s="4">
-        <f>BC13*(1+$AK21)</f>
-        <v>63.808627540172068</v>
+        <f t="shared" si="21"/>
+        <v>14.44592491316194</v>
       </c>
       <c r="BE13" s="4">
-        <f>BD13*(1+$AK21)</f>
-        <v>63.17054126477035</v>
+        <f t="shared" si="21"/>
+        <v>14.301465664030321</v>
       </c>
       <c r="BF13" s="4">
-        <f>BE13*(1+$AK21)</f>
-        <v>62.538835852122645</v>
+        <f t="shared" si="21"/>
+        <v>14.158451007390017</v>
       </c>
       <c r="BG13" s="4">
-        <f>BF13*(1+$AK21)</f>
-        <v>61.913447493601417</v>
+        <f t="shared" si="21"/>
+        <v>14.016866497316117</v>
       </c>
       <c r="BH13" s="4">
-        <f>BG13*(1+$AK21)</f>
-        <v>61.294313018665406</v>
+        <f t="shared" si="21"/>
+        <v>13.876697832342956</v>
       </c>
       <c r="BI13" s="4">
-        <f>BH13*(1+$AK21)</f>
-        <v>60.681369888478748</v>
+        <f t="shared" si="21"/>
+        <v>13.737930854019526</v>
       </c>
       <c r="BJ13" s="4">
-        <f>BI13*(1+$AK21)</f>
-        <v>60.074556189593963</v>
+        <f t="shared" si="21"/>
+        <v>13.60055154547933</v>
       </c>
       <c r="BK13" s="4">
-        <f>BJ13*(1+$AK21)</f>
-        <v>59.473810627698022</v>
+        <f t="shared" si="21"/>
+        <v>13.464546030024538</v>
       </c>
       <c r="BL13" s="4">
-        <f>BK13*(1+$AK21)</f>
-        <v>58.879072521421044</v>
+        <f t="shared" si="21"/>
+        <v>13.329900569724293</v>
       </c>
       <c r="BM13" s="4">
-        <f>BL13*(1+$AK21)</f>
-        <v>58.290281796206834</v>
+        <f t="shared" si="21"/>
+        <v>13.19660156402705</v>
       </c>
       <c r="BN13" s="4">
-        <f>BM13*(1+$AK21)</f>
-        <v>57.707378978244762</v>
+        <f t="shared" ref="BN13:CS13" si="22">BM13*(1+$AK21)</f>
+        <v>13.06463554838678</v>
       </c>
       <c r="BO13" s="4">
-        <f>BN13*(1+$AK21)</f>
-        <v>57.130305188462316</v>
+        <f t="shared" si="22"/>
+        <v>12.933989192902912</v>
       </c>
       <c r="BP13" s="4">
-        <f>BO13*(1+$AK21)</f>
-        <v>56.559002136577689</v>
+        <f t="shared" si="22"/>
+        <v>12.804649300973882</v>
       </c>
       <c r="BQ13" s="4">
-        <f>BP13*(1+$AK21)</f>
-        <v>55.99341211521191</v>
+        <f t="shared" si="22"/>
+        <v>12.676602807964143</v>
       </c>
       <c r="BR13" s="4">
-        <f>BQ13*(1+$AK21)</f>
-        <v>55.433477994059793</v>
+        <f t="shared" si="22"/>
+        <v>12.549836779884501</v>
       </c>
       <c r="BS13" s="4">
-        <f>BR13*(1+$AK21)</f>
-        <v>54.879143214119196</v>
+        <f t="shared" si="22"/>
+        <v>12.424338412085655</v>
       </c>
       <c r="BT13" s="4">
-        <f>BS13*(1+$AK21)</f>
-        <v>54.330351781978003</v>
+        <f t="shared" si="22"/>
+        <v>12.300095027964799</v>
       </c>
       <c r="BU13" s="4">
-        <f>BT13*(1+$AK21)</f>
-        <v>53.787048264158223</v>
+        <f t="shared" si="22"/>
+        <v>12.177094077685151</v>
       </c>
       <c r="BV13" s="4">
-        <f>BU13*(1+$AK21)</f>
-        <v>53.249177781516643</v>
+        <f t="shared" si="22"/>
+        <v>12.055323136908299</v>
       </c>
       <c r="BW13" s="4">
-        <f>BV13*(1+$AK21)</f>
-        <v>52.716686003701476</v>
+        <f t="shared" si="22"/>
+        <v>11.934769905539216</v>
       </c>
       <c r="BX13" s="4">
-        <f>BW13*(1+$AK21)</f>
-        <v>52.189519143664462</v>
+        <f t="shared" si="22"/>
+        <v>11.815422206483824</v>
       </c>
       <c r="BY13" s="4">
-        <f>BX13*(1+$AK21)</f>
-        <v>51.667623952227814</v>
+        <f t="shared" si="22"/>
+        <v>11.697267984418986</v>
       </c>
       <c r="BZ13" s="4">
-        <f>BY13*(1+$AK21)</f>
-        <v>51.150947712705538</v>
+        <f t="shared" si="22"/>
+        <v>11.580295304574795</v>
       </c>
       <c r="CA13" s="4">
-        <f>BZ13*(1+$AK21)</f>
-        <v>50.639438235578481</v>
+        <f t="shared" si="22"/>
+        <v>11.464492351529048</v>
       </c>
       <c r="CB13" s="4">
-        <f>CA13*(1+$AK21)</f>
-        <v>50.133043853222695</v>
+        <f t="shared" si="22"/>
+        <v>11.349847428013756</v>
       </c>
       <c r="CC13" s="4">
-        <f>CB13*(1+$AK21)</f>
-        <v>49.631713414690466</v>
+        <f t="shared" si="22"/>
+        <v>11.23634895373362</v>
       </c>
       <c r="CD13" s="4">
-        <f>CC13*(1+$AK21)</f>
-        <v>49.13539628054356</v>
+        <f t="shared" si="22"/>
+        <v>11.123985464196283</v>
       </c>
       <c r="CE13" s="4">
-        <f>CD13*(1+$AK21)</f>
-        <v>48.644042317738126</v>
+        <f t="shared" si="22"/>
+        <v>11.012745609554319</v>
       </c>
       <c r="CF13" s="4">
-        <f>CE13*(1+$AK21)</f>
-        <v>48.157601894560742</v>
+        <f t="shared" si="22"/>
+        <v>10.902618153458775</v>
       </c>
       <c r="CG13" s="4">
-        <f>CF13*(1+$AK21)</f>
-        <v>47.676025875615132</v>
+        <f t="shared" si="22"/>
+        <v>10.793591971924187</v>
       </c>
       <c r="CH13" s="4">
-        <f>CG13*(1+$AK21)</f>
-        <v>47.19926561685898</v>
+        <f t="shared" si="22"/>
+        <v>10.685656052204944</v>
       </c>
       <c r="CI13" s="4">
-        <f>CH13*(1+$AK21)</f>
-        <v>46.727272960690392</v>
+        <f t="shared" si="22"/>
+        <v>10.578799491682895</v>
       </c>
       <c r="CJ13" s="4">
-        <f>CI13*(1+$AK21)</f>
-        <v>46.260000231083488</v>
+        <f t="shared" si="22"/>
+        <v>10.473011496766066</v>
       </c>
       <c r="CK13" s="4">
-        <f>CJ13*(1+$AK21)</f>
-        <v>45.797400228772652</v>
+        <f t="shared" si="22"/>
+        <v>10.368281381798406</v>
       </c>
       <c r="CL13" s="4">
-        <f>CK13*(1+$AK21)</f>
-        <v>45.339426226484925</v>
+        <f t="shared" si="22"/>
+        <v>10.264598567980421</v>
       </c>
       <c r="CM13" s="4">
-        <f>CL13*(1+$AK21)</f>
-        <v>44.886031964220074</v>
+        <f t="shared" si="22"/>
+        <v>10.161952582300618</v>
       </c>
       <c r="CN13" s="4">
-        <f>CM13*(1+$AK21)</f>
-        <v>44.437171644577873</v>
+        <f t="shared" si="22"/>
+        <v>10.060333056477612</v>
       </c>
       <c r="CO13" s="4">
-        <f>CN13*(1+$AK21)</f>
-        <v>43.992799928132094</v>
+        <f t="shared" si="22"/>
+        <v>9.959729725912835</v>
       </c>
       <c r="CP13" s="4">
-        <f>CO13*(1+$AK21)</f>
-        <v>43.55287192885077</v>
+        <f t="shared" si="22"/>
+        <v>9.8601324286537064</v>
       </c>
       <c r="CQ13" s="4">
-        <f>CP13*(1+$AK21)</f>
-        <v>43.117343209562264</v>
+        <f t="shared" si="22"/>
+        <v>9.7615311043671689</v>
       </c>
       <c r="CR13" s="4">
-        <f>CQ13*(1+$AK21)</f>
-        <v>42.686169777466638</v>
+        <f t="shared" si="22"/>
+        <v>9.6639157933234969</v>
       </c>
       <c r="CS13" s="4">
-        <f>CR13*(1+$AK21)</f>
-        <v>42.259308079691969</v>
+        <f t="shared" si="22"/>
+        <v>9.5672766353902627</v>
       </c>
       <c r="CT13" s="4">
-        <f>CS13*(1+$AK21)</f>
-        <v>41.836714998895047</v>
+        <f t="shared" ref="CT13:DY13" si="23">CS13*(1+$AK21)</f>
+        <v>9.4716038690363593</v>
       </c>
       <c r="CU13" s="4">
-        <f>CT13*(1+$AK21)</f>
-        <v>41.418347848906095</v>
+        <f t="shared" si="23"/>
+        <v>9.3768878303459964</v>
       </c>
       <c r="CV13" s="4">
-        <f>CU13*(1+$AK21)</f>
-        <v>41.00416437041703</v>
+        <f t="shared" si="23"/>
+        <v>9.2831189520425355</v>
       </c>
       <c r="CW13" s="4">
-        <f>CV13*(1+$AK21)</f>
-        <v>40.594122726712861</v>
+        <f t="shared" si="23"/>
+        <v>9.1902877625221109</v>
       </c>
       <c r="CX13" s="4">
-        <f>CW13*(1+$AK21)</f>
-        <v>40.188181499445733</v>
+        <f t="shared" si="23"/>
+        <v>9.0983848848968893</v>
       </c>
       <c r="CY13" s="4">
-        <f>CX13*(1+$AK21)</f>
-        <v>39.786299684451272</v>
+        <f t="shared" si="23"/>
+        <v>9.00740103604792</v>
       </c>
       <c r="CZ13" s="4">
-        <f>CY13*(1+$AK21)</f>
-        <v>39.388436687606756</v>
+        <f t="shared" si="23"/>
+        <v>8.91732702568744</v>
       </c>
       <c r="DA13" s="4">
-        <f>CZ13*(1+$AK21)</f>
-        <v>38.994552320730691</v>
+        <f t="shared" si="23"/>
+        <v>8.8281537554305647</v>
       </c>
       <c r="DB13" s="4">
-        <f>DA13*(1+$AK21)</f>
-        <v>38.604606797523381</v>
+        <f t="shared" si="23"/>
+        <v>8.7398722178762593</v>
       </c>
       <c r="DC13" s="4">
-        <f>DB13*(1+$AK21)</f>
-        <v>38.218560729548145</v>
+        <f t="shared" si="23"/>
+        <v>8.652473495697496</v>
       </c>
       <c r="DD13" s="4">
-        <f>DC13*(1+$AK21)</f>
-        <v>37.836375122252662</v>
+        <f t="shared" si="23"/>
+        <v>8.5659487607405218</v>
       </c>
       <c r="DE13" s="4">
-        <f>DD13*(1+$AK21)</f>
-        <v>37.458011371030132</v>
+        <f t="shared" si="23"/>
+        <v>8.480289273133117</v>
       </c>
       <c r="DF13" s="4">
-        <f>DE13*(1+$AK21)</f>
-        <v>37.08343125731983</v>
+        <f t="shared" si="23"/>
+        <v>8.3954863804017865</v>
       </c>
       <c r="DG13" s="4">
-        <f>DF13*(1+$AK21)</f>
-        <v>36.712596944746629</v>
+        <f t="shared" si="23"/>
+        <v>8.3115315165977695</v>
       </c>
       <c r="DH13" s="4">
-        <f>DG13*(1+$AK21)</f>
-        <v>36.345470975299165</v>
+        <f t="shared" si="23"/>
+        <v>8.2284162014317914</v>
       </c>
       <c r="DI13" s="4">
-        <f>DH13*(1+$AK21)</f>
-        <v>35.982016265546171</v>
+        <f t="shared" si="23"/>
+        <v>8.1461320394174734</v>
       </c>
       <c r="DJ13" s="4">
-        <f>DI13*(1+$AK21)</f>
-        <v>35.622196102890712</v>
+        <f t="shared" si="23"/>
+        <v>8.0646707190232991</v>
       </c>
       <c r="DK13" s="4">
-        <f>DJ13*(1+$AK21)</f>
-        <v>35.265974141861804</v>
+        <f t="shared" si="23"/>
+        <v>7.9840240118330659</v>
       </c>
       <c r="DL13" s="4">
-        <f>DK13*(1+$AK21)</f>
-        <v>34.913314400443184</v>
+        <f t="shared" si="23"/>
+        <v>7.9041837717147354</v>
       </c>
       <c r="DM13" s="4">
-        <f>DL13*(1+$AK21)</f>
-        <v>34.564181256438751</v>
+        <f t="shared" si="23"/>
+        <v>7.8251419339975881</v>
       </c>
       <c r="DN13" s="4">
-        <f>DM13*(1+$AK21)</f>
-        <v>34.218539443874363</v>
+        <f t="shared" si="23"/>
+        <v>7.7468905146576121</v>
       </c>
       <c r="DO13" s="4">
-        <f>DN13*(1+$AK21)</f>
-        <v>33.876354049435619</v>
+        <f t="shared" si="23"/>
+        <v>7.6694216095110361</v>
       </c>
       <c r="DP13" s="4">
-        <f>DO13*(1+$AK21)</f>
-        <v>33.537590508941264</v>
+        <f t="shared" si="23"/>
+        <v>7.5927273934159256</v>
       </c>
       <c r="DQ13" s="4">
-        <f>DP13*(1+$AK21)</f>
-        <v>33.20221460385185</v>
+        <f t="shared" si="23"/>
+        <v>7.5168001194817666</v>
       </c>
       <c r="DR13" s="4">
-        <f>DQ13*(1+$AK21)</f>
-        <v>32.870192457813332</v>
+        <f t="shared" si="23"/>
+        <v>7.4416321182869485</v>
       </c>
       <c r="DS13" s="4">
-        <f>DR13*(1+$AK21)</f>
-        <v>32.541490533235198</v>
+        <f t="shared" si="23"/>
+        <v>7.3672157971040786</v>
       </c>
       <c r="DT13" s="4">
-        <f>DS13*(1+$AK21)</f>
-        <v>32.216075627902846</v>
+        <f t="shared" si="23"/>
+        <v>7.2935436391330377</v>
       </c>
       <c r="DU13" s="4">
-        <f>DT13*(1+$AK21)</f>
-        <v>31.893914871623817</v>
+        <f t="shared" si="23"/>
+        <v>7.2206082027417073</v>
       </c>
       <c r="DV13" s="4">
-        <f>DU13*(1+$AK21)</f>
-        <v>31.574975722907578</v>
+        <f t="shared" si="23"/>
+        <v>7.14840212071429</v>
       </c>
       <c r="DW13" s="4">
-        <f>DV13*(1+$AK21)</f>
-        <v>31.259225965678503</v>
+        <f t="shared" si="23"/>
+        <v>7.0769180995071475</v>
       </c>
       <c r="DX13" s="4">
-        <f>DW13*(1+$AK21)</f>
-        <v>30.946633706021718</v>
+        <f t="shared" si="23"/>
+        <v>7.0061489185120758</v>
       </c>
       <c r="DY13" s="4">
-        <f>DX13*(1+$AK21)</f>
-        <v>30.637167368961499</v>
+        <f t="shared" si="23"/>
+        <v>6.936087429326955</v>
       </c>
       <c r="DZ13" s="4">
-        <f>DY13*(1+$AK21)</f>
-        <v>30.330795695271885</v>
+        <f t="shared" ref="DZ13:FE13" si="24">DY13*(1+$AK21)</f>
+        <v>6.8667265550336856</v>
       </c>
       <c r="EA13" s="4">
-        <f>DZ13*(1+$AK21)</f>
-        <v>30.027487738319167</v>
+        <f t="shared" si="24"/>
+        <v>6.7980592894833487</v>
       </c>
       <c r="EB13" s="4">
-        <f>EA13*(1+$AK21)</f>
-        <v>29.727212860935975</v>
+        <f t="shared" si="24"/>
+        <v>6.7300786965885155</v>
       </c>
       <c r="EC13" s="4">
-        <f>EB13*(1+$AK21)</f>
-        <v>29.429940732326614</v>
+        <f t="shared" si="24"/>
+        <v>6.6627779096226307</v>
       </c>
       <c r="ED13" s="4">
-        <f>EC13*(1+$AK21)</f>
-        <v>29.135641325003348</v>
+        <f t="shared" si="24"/>
+        <v>6.5961501305264045</v>
       </c>
       <c r="EE13" s="4">
-        <f>ED13*(1+$AK21)</f>
-        <v>28.844284911753313</v>
+        <f t="shared" si="24"/>
+        <v>6.5301886292211409</v>
       </c>
       <c r="EF13" s="4">
-        <f>EE13*(1+$AK21)</f>
-        <v>28.555842062635779</v>
+        <f t="shared" si="24"/>
+        <v>6.464886742928929</v>
       </c>
       <c r="EG13" s="4">
-        <f>EF13*(1+$AK21)</f>
-        <v>28.270283642009421</v>
+        <f t="shared" si="24"/>
+        <v>6.4002378754996396</v>
       </c>
       <c r="EH13" s="4">
-        <f>EG13*(1+$AK21)</f>
-        <v>27.987580805589328</v>
+        <f t="shared" si="24"/>
+        <v>6.336235496744643</v>
       </c>
       <c r="EI13" s="4">
-        <f>EH13*(1+$AK21)</f>
-        <v>27.707704997533433</v>
+        <f t="shared" si="24"/>
+        <v>6.2728731417771968</v>
       </c>
       <c r="EJ13" s="4">
-        <f>EI13*(1+$AK21)</f>
-        <v>27.430627947558097</v>
+        <f t="shared" si="24"/>
+        <v>6.2101444103594243</v>
       </c>
       <c r="EK13" s="4">
-        <f>EJ13*(1+$AK21)</f>
-        <v>27.156321668082516</v>
+        <f t="shared" si="24"/>
+        <v>6.1480429662558302</v>
       </c>
       <c r="EL13" s="4">
-        <f>EK13*(1+$AK21)</f>
-        <v>26.884758451401691</v>
+        <f t="shared" si="24"/>
+        <v>6.0865625365932718</v>
       </c>
       <c r="EM13" s="4">
-        <f>EL13*(1+$AK21)</f>
-        <v>26.615910866887674</v>
+        <f t="shared" si="24"/>
+        <v>6.0256969112273389</v>
       </c>
       <c r="EN13" s="4">
-        <f>EM13*(1+$AK21)</f>
-        <v>26.349751758218797</v>
+        <f t="shared" si="24"/>
+        <v>5.965439942115065</v>
       </c>
       <c r="EO13" s="4">
-        <f>EN13*(1+$AK21)</f>
-        <v>26.08625424063661</v>
+        <f t="shared" si="24"/>
+        <v>5.9057855426939145</v>
       </c>
       <c r="EP13" s="4">
-        <f>EO13*(1+$AK21)</f>
-        <v>25.825391698230245</v>
+        <f t="shared" si="24"/>
+        <v>5.8467276872669753</v>
       </c>
       <c r="EQ13" s="4">
-        <f>EP13*(1+$AK21)</f>
-        <v>25.567137781247943</v>
+        <f t="shared" si="24"/>
+        <v>5.7882604103943054</v>
       </c>
       <c r="ER13" s="4">
-        <f>EQ13*(1+$AK21)</f>
-        <v>25.311466403435464</v>
+        <f t="shared" si="24"/>
+        <v>5.7303778062903623</v>
       </c>
       <c r="ES13" s="4">
-        <f>ER13*(1+$AK21)</f>
-        <v>25.058351739401107</v>
+        <f t="shared" si="24"/>
+        <v>5.6730740282274583</v>
       </c>
       <c r="ET13" s="4">
-        <f>ES13*(1+$AK21)</f>
-        <v>24.807768222007095</v>
+        <f t="shared" si="24"/>
+        <v>5.6163432879451838</v>
       </c>
       <c r="EU13" s="4">
-        <f>ET13*(1+$AK21)</f>
-        <v>24.559690539787024</v>
+        <f t="shared" si="24"/>
+        <v>5.5601798550657318</v>
       </c>
       <c r="EV13" s="4">
-        <f>EU13*(1+$AK21)</f>
-        <v>24.314093634389152</v>
+        <f t="shared" si="24"/>
+        <v>5.5045780565150748</v>
       </c>
       <c r="EW13" s="4">
-        <f>EV13*(1+$AK21)</f>
-        <v>24.070952698045261</v>
+        <f t="shared" si="24"/>
+        <v>5.4495322759499238</v>
       </c>
       <c r="EX13" s="4">
-        <f>EW13*(1+$AK21)</f>
-        <v>23.830243171064808</v>
+        <f t="shared" si="24"/>
+        <v>5.3950369531904245</v>
       </c>
       <c r="EY13" s="4">
-        <f>EX13*(1+$AK21)</f>
-        <v>23.591940739354161</v>
+        <f t="shared" si="24"/>
+        <v>5.3410865836585204</v>
       </c>
       <c r="EZ13" s="4">
-        <f>EY13*(1+$AK21)</f>
-        <v>23.356021331960619</v>
+        <f t="shared" si="24"/>
+        <v>5.2876757178219354</v>
       </c>
       <c r="FA13" s="4">
-        <f>EZ13*(1+$AK21)</f>
-        <v>23.122461118641013</v>
+        <f t="shared" si="24"/>
+        <v>5.2347989606437162</v>
       </c>
       <c r="FB13" s="4">
-        <f>FA13*(1+$AK21)</f>
-        <v>22.891236507454604</v>
+        <f t="shared" si="24"/>
+        <v>5.1824509710372793</v>
       </c>
       <c r="FC13" s="4">
-        <f>FB13*(1+$AK21)</f>
-        <v>22.662324142380058</v>
+        <f t="shared" si="24"/>
+        <v>5.1306264613269068</v>
       </c>
       <c r="FD13" s="4">
-        <f>FC13*(1+$AK21)</f>
-        <v>22.435700900956256</v>
+        <f t="shared" si="24"/>
+        <v>5.0793201967136374</v>
       </c>
       <c r="FE13" s="4">
-        <f>FD13*(1+$AK21)</f>
-        <v>22.211343891946694</v>
+        <f t="shared" si="24"/>
+        <v>5.0285269947465014</v>
       </c>
       <c r="FF13" s="4">
-        <f>FE13*(1+$AK21)</f>
-        <v>21.989230453027226</v>
+        <f t="shared" ref="FF13:GK13" si="25">FE13*(1+$AK21)</f>
+        <v>4.9782417247990365</v>
       </c>
       <c r="FG13" s="4">
-        <f>FF13*(1+$AK21)</f>
-        <v>21.769338148496953</v>
+        <f t="shared" si="25"/>
+        <v>4.9284593075510461</v>
       </c>
       <c r="FH13" s="4">
-        <f>FG13*(1+$AK21)</f>
-        <v>21.551644767011982</v>
+        <f t="shared" si="25"/>
+        <v>4.8791747144755355</v>
       </c>
       <c r="FI13" s="4">
-        <f>FH13*(1+$AK21)</f>
-        <v>21.336128319341864</v>
+        <f t="shared" si="25"/>
+        <v>4.8303829673307801</v>
       </c>
       <c r="FJ13" s="4">
-        <f>FI13*(1+$AK21)</f>
-        <v>21.122767036148446</v>
+        <f t="shared" si="25"/>
+        <v>4.7820791376574725</v>
       </c>
       <c r="FK13" s="4">
-        <f>FJ13*(1+$AK21)</f>
-        <v>20.911539365786961</v>
+        <f t="shared" si="25"/>
+        <v>4.7342583462808978</v>
       </c>
       <c r="FL13" s="4">
-        <f>FK13*(1+$AK21)</f>
-        <v>20.70242397212909</v>
+        <f t="shared" si="25"/>
+        <v>4.6869157628180886</v>
       </c>
       <c r="FM13" s="4">
-        <f>FL13*(1+$AK21)</f>
-        <v>20.495399732407797</v>
+        <f t="shared" si="25"/>
+        <v>4.6400466051899079</v>
       </c>
       <c r="FN13" s="4">
-        <f>FM13*(1+$AK21)</f>
-        <v>20.290445735083718</v>
+        <f t="shared" si="25"/>
+        <v>4.5936461391380083</v>
       </c>
       <c r="FO13" s="4">
-        <f>FN13*(1+$AK21)</f>
-        <v>20.087541277732882</v>
+        <f t="shared" si="25"/>
+        <v>4.5477096777466279</v>
       </c>
       <c r="FP13" s="4">
-        <f>FO13*(1+$AK21)</f>
-        <v>19.886665864955553</v>
+        <f t="shared" si="25"/>
+        <v>4.5022325809691619</v>
       </c>
       <c r="FQ13" s="4">
-        <f>FP13*(1+$AK21)</f>
-        <v>19.687799206305996</v>
+        <f t="shared" si="25"/>
+        <v>4.4572102551594703</v>
       </c>
       <c r="FR13" s="4">
-        <f>FQ13*(1+$AK21)</f>
-        <v>19.490921214242935</v>
+        <f t="shared" si="25"/>
+        <v>4.412638152607876</v>
       </c>
       <c r="FS13" s="4">
-        <f>FR13*(1+$AK21)</f>
-        <v>19.296012002100504</v>
+        <f t="shared" si="25"/>
+        <v>4.3685117710817973</v>
       </c>
       <c r="FT13" s="4">
-        <f>FS13*(1+$AK21)</f>
-        <v>19.103051882079498</v>
+        <f t="shared" si="25"/>
+        <v>4.3248266533709794</v>
       </c>
       <c r="FU13" s="4">
-        <f>FT13*(1+$AK21)</f>
-        <v>18.912021363258702</v>
+        <f t="shared" si="25"/>
+        <v>4.2815783868372694</v>
       </c>
       <c r="FV13" s="4">
-        <f>FU13*(1+$AK21)</f>
-        <v>18.722901149626114</v>
+        <f t="shared" si="25"/>
+        <v>4.2387626029688965</v>
       </c>
       <c r="FW13" s="4">
-        <f>FV13*(1+$AK21)</f>
-        <v>18.535672138129854</v>
+        <f t="shared" si="25"/>
+        <v>4.1963749769392074</v>
       </c>
       <c r="FX13" s="4">
-        <f>FW13*(1+$AK21)</f>
-        <v>18.350315416748554</v>
+        <f t="shared" si="25"/>
+        <v>4.154411227169815</v>
       </c>
       <c r="FY13" s="4">
-        <f>FX13*(1+$AK21)</f>
-        <v>18.166812262581068</v>
+        <f t="shared" si="25"/>
+        <v>4.1128671148981164</v>
       </c>
       <c r="FZ13" s="4">
-        <f>FY13*(1+$AK21)</f>
-        <v>17.985144139955256</v>
+        <f t="shared" si="25"/>
+        <v>4.0717384437491351</v>
       </c>
       <c r="GA13" s="4">
-        <f>FZ13*(1+$AK21)</f>
-        <v>17.805292698555704</v>
+        <f t="shared" si="25"/>
+        <v>4.0310210593116436</v>
       </c>
       <c r="GB13" s="4">
-        <f>GA13*(1+$AK21)</f>
-        <v>17.627239771570146</v>
+        <f t="shared" si="25"/>
+        <v>3.990710848718527</v>
       </c>
       <c r="GC13" s="4">
-        <f>GB13*(1+$AK21)</f>
-        <v>17.450967373854443</v>
+        <f t="shared" si="25"/>
+        <v>3.9508037402313416</v>
       </c>
       <c r="GD13" s="4">
-        <f>GC13*(1+$AK21)</f>
-        <v>17.276457700115898</v>
+        <f t="shared" si="25"/>
+        <v>3.9112957028290283</v>
       </c>
       <c r="GE13" s="4">
-        <f>GD13*(1+$AK21)</f>
-        <v>17.103693123114738</v>
+        <f t="shared" si="25"/>
+        <v>3.8721827458007381</v>
       </c>
       <c r="GF13" s="4">
-        <f>GE13*(1+$AK21)</f>
-        <v>16.932656191883591</v>
+        <f t="shared" si="25"/>
+        <v>3.8334609183427308</v>
       </c>
       <c r="GG13" s="4">
-        <f>GF13*(1+$AK21)</f>
-        <v>16.763329629964755</v>
+        <f t="shared" si="25"/>
+        <v>3.7951263091593037</v>
       </c>
       <c r="GH13" s="4">
-        <f>GG13*(1+$AK21)</f>
-        <v>16.595696333665106</v>
+        <f t="shared" si="25"/>
+        <v>3.7571750460677107</v>
       </c>
       <c r="GI13" s="4">
-        <f>GH13*(1+$AK21)</f>
-        <v>16.429739370328456</v>
+        <f t="shared" si="25"/>
+        <v>3.7196032956070337</v>
       </c>
       <c r="GJ13" s="4">
-        <f>GI13*(1+$AK21)</f>
-        <v>16.265441976625169</v>
+        <f t="shared" si="25"/>
+        <v>3.6824072626509632</v>
       </c>
       <c r="GK13" s="4">
-        <f>GJ13*(1+$AK21)</f>
-        <v>16.102787556858917</v>
+        <f t="shared" si="25"/>
+        <v>3.6455831900244533</v>
       </c>
       <c r="GL13" s="4">
-        <f>GK13*(1+$AK21)</f>
-        <v>15.941759681290328</v>
+        <f t="shared" ref="GL13:HH13" si="26">GK13*(1+$AK21)</f>
+        <v>3.6091273581242089</v>
       </c>
       <c r="GM13" s="4">
-        <f>GL13*(1+$AK21)</f>
-        <v>15.782342084477426</v>
+        <f t="shared" si="26"/>
+        <v>3.573036084542967</v>
       </c>
       <c r="GN13" s="4">
-        <f>GM13*(1+$AK21)</f>
-        <v>15.624518663632651</v>
+        <f t="shared" si="26"/>
+        <v>3.5373057236975374</v>
       </c>
       <c r="GO13" s="4">
-        <f>GN13*(1+$AK21)</f>
-        <v>15.468273476996325</v>
+        <f t="shared" si="26"/>
+        <v>3.5019326664605619</v>
       </c>
       <c r="GP13" s="4">
-        <f>GO13*(1+$AK21)</f>
-        <v>15.313590742226362</v>
+        <f t="shared" si="26"/>
+        <v>3.4669133397959562</v>
       </c>
       <c r="GQ13" s="4">
-        <f>GP13*(1+$AK21)</f>
-        <v>15.160454834804098</v>
+        <f t="shared" si="26"/>
+        <v>3.4322442063979968</v>
       </c>
       <c r="GR13" s="4">
-        <f>GQ13*(1+$AK21)</f>
-        <v>15.008850286456056</v>
+        <f t="shared" si="26"/>
+        <v>3.3979217643340167</v>
       </c>
       <c r="GS13" s="4">
-        <f>GR13*(1+$AK21)</f>
-        <v>14.858761783591495</v>
+        <f t="shared" si="26"/>
+        <v>3.3639425466906765</v>
       </c>
       <c r="GT13" s="4">
-        <f>GS13*(1+$AK21)</f>
-        <v>14.71017416575558</v>
+        <f t="shared" si="26"/>
+        <v>3.3303031212237695</v>
       </c>
       <c r="GU13" s="4">
-        <f>GT13*(1+$AK21)</f>
-        <v>14.563072424098024</v>
+        <f t="shared" si="26"/>
+        <v>3.2970000900115317</v>
       </c>
       <c r="GV13" s="4">
-        <f>GU13*(1+$AK21)</f>
-        <v>14.417441699857044</v>
+        <f t="shared" si="26"/>
+        <v>3.2640300891114165</v>
       </c>
       <c r="GW13" s="4">
-        <f>GV13*(1+$AK21)</f>
-        <v>14.273267282858473</v>
+        <f t="shared" si="26"/>
+        <v>3.2313897882203024</v>
       </c>
       <c r="GX13" s="4">
-        <f>GW13*(1+$AK21)</f>
-        <v>14.130534610029889</v>
+        <f t="shared" si="26"/>
+        <v>3.1990758903380994</v>
       </c>
       <c r="GY13" s="4">
-        <f>GX13*(1+$AK21)</f>
-        <v>13.989229263929589</v>
+        <f t="shared" si="26"/>
+        <v>3.1670851314347184</v>
       </c>
       <c r="GZ13" s="4">
-        <f>GY13*(1+$AK21)</f>
-        <v>13.849336971290294</v>
+        <f t="shared" si="26"/>
+        <v>3.1354142801203713</v>
       </c>
       <c r="HA13" s="4">
-        <f>GZ13*(1+$AK21)</f>
-        <v>13.710843601577391</v>
+        <f t="shared" si="26"/>
+        <v>3.1040601373191676</v>
       </c>
       <c r="HB13" s="4">
-        <f>HA13*(1+$AK21)</f>
-        <v>13.573735165561617</v>
+        <f t="shared" si="26"/>
+        <v>3.073019535945976</v>
       </c>
       <c r="HC13" s="4">
-        <f>HB13*(1+$AK21)</f>
-        <v>13.437997813906001</v>
+        <f t="shared" si="26"/>
+        <v>3.0422893405865161</v>
       </c>
       <c r="HD13" s="4">
-        <f>HC13*(1+$AK21)</f>
-        <v>13.303617835766941</v>
+        <f t="shared" si="26"/>
+        <v>3.0118664471806511</v>
       </c>
       <c r="HE13" s="4">
-        <f>HD13*(1+$AK21)</f>
-        <v>13.170581657409272</v>
+        <f t="shared" si="26"/>
+        <v>2.9817477827088448</v>
       </c>
       <c r="HF13" s="4">
-        <f>HE13*(1+$AK21)</f>
-        <v>13.03887584083518</v>
+        <f t="shared" si="26"/>
+        <v>2.9519303048817562</v>
       </c>
       <c r="HG13" s="4">
-        <f>HF13*(1+$AK21)</f>
-        <v>12.908487082426829</v>
+        <f t="shared" si="26"/>
+        <v>2.9224110018329386</v>
       </c>
       <c r="HH13" s="4">
-        <f>HG13*(1+$AK21)</f>
-        <v>12.779402211602561</v>
+        <f t="shared" si="26"/>
+        <v>2.8931868918146093</v>
       </c>
     </row>
     <row r="14" spans="2:216" s="3" customFormat="1" x14ac:dyDescent="0.25">
@@ -3186,8 +3259,12 @@
       <c r="K14" s="5">
         <v>13.874000000000001</v>
       </c>
-      <c r="L14" s="4"/>
-      <c r="M14" s="4"/>
+      <c r="L14" s="5">
+        <v>13.93</v>
+      </c>
+      <c r="M14" s="5">
+        <v>13.962</v>
+      </c>
       <c r="N14" s="4"/>
       <c r="P14" s="12"/>
       <c r="Q14" s="4"/>
@@ -3402,57 +3479,63 @@
         <v>23</v>
       </c>
       <c r="C15" s="16">
-        <f t="shared" ref="C15" si="12">C13/C14</f>
+        <f t="shared" ref="C15" si="27">C13/C14</f>
         <v>-1.5826801801801802</v>
       </c>
       <c r="D15" s="16">
-        <f t="shared" ref="D15:K15" si="13">D13/D14</f>
+        <f t="shared" ref="D15:K15" si="28">D13/D14</f>
         <v>-2.1256562046241489</v>
       </c>
       <c r="E15" s="16">
-        <f t="shared" si="13"/>
+        <f t="shared" si="28"/>
         <v>-2.5002860302810732</v>
       </c>
       <c r="F15" s="16">
-        <f t="shared" si="13"/>
+        <f t="shared" si="28"/>
         <v>-2.8011236492003744</v>
       </c>
       <c r="G15" s="16">
-        <f t="shared" si="13"/>
+        <f t="shared" si="28"/>
         <v>-1.8901656314699777</v>
       </c>
       <c r="H15" s="16">
-        <f t="shared" si="13"/>
+        <f t="shared" si="28"/>
         <v>-1.9795180722891563</v>
       </c>
       <c r="I15" s="16">
-        <f t="shared" si="13"/>
+        <f t="shared" si="28"/>
         <v>0.81435607706793944</v>
       </c>
       <c r="J15" s="16">
-        <f t="shared" si="13"/>
+        <f t="shared" si="28"/>
         <v>0.25880052151238669</v>
       </c>
       <c r="K15" s="16">
-        <f t="shared" si="13"/>
+        <f t="shared" si="28"/>
         <v>1.0385613377540726</v>
       </c>
-      <c r="L15" s="16"/>
-      <c r="M15" s="16"/>
+      <c r="L15" s="16">
+        <f t="shared" ref="L15:M15" si="29">L13/L14</f>
+        <v>1.2778894472361806</v>
+      </c>
+      <c r="M15" s="16">
+        <f t="shared" si="29"/>
+        <v>0.63887695172611136</v>
+      </c>
       <c r="N15" s="16"/>
       <c r="P15" s="18"/>
       <c r="Q15" s="16"/>
       <c r="T15" s="16">
-        <f t="shared" ref="T15:W15" si="14">T13/T14</f>
+        <f t="shared" ref="T15:V15" si="30">T13/T14</f>
         <v>-14.462308509024723</v>
       </c>
       <c r="U15" s="16">
-        <f t="shared" si="14"/>
+        <f t="shared" si="30"/>
         <v>-2.0344777632913225</v>
       </c>
       <c r="V15" s="16">
-        <f t="shared" si="14"/>
-        <v>2.1505832246849179</v>
+        <f t="shared" si="30"/>
+        <v>3.2882697377951589</v>
       </c>
       <c r="W15" s="16"/>
       <c r="X15" s="16"/>
@@ -3628,52 +3711,52 @@
         <v>-173.79999999999998</v>
       </c>
       <c r="V19" s="5">
-        <f>U19+U13</f>
+        <f t="shared" ref="V19:AG19" si="31">U19+U13</f>
         <v>-201.88799999999998</v>
       </c>
       <c r="W19" s="5">
-        <f>V19+V13</f>
-        <v>-172.197048</v>
+        <f t="shared" si="31"/>
+        <v>-156.49014800000003</v>
       </c>
       <c r="X19" s="5">
-        <f>W19+W13</f>
-        <v>-128.77702260000001</v>
+        <f t="shared" si="31"/>
+        <v>-158.05154282000007</v>
       </c>
       <c r="Y19" s="5">
-        <f>X19+X13</f>
-        <v>-69.091100452199953</v>
+        <f t="shared" si="31"/>
+        <v>-140.42133233610005</v>
       </c>
       <c r="Z19" s="5">
-        <f>Y19+Y13</f>
-        <v>9.7582003875751013</v>
+        <f t="shared" si="31"/>
+        <v>-119.22866862739055</v>
       </c>
       <c r="AA19" s="5">
-        <f>Z19+Z13</f>
-        <v>110.19613318775264</v>
+        <f t="shared" si="31"/>
+        <v>-74.40418904052143</v>
       </c>
       <c r="AB19" s="5">
-        <f>AA19+AA13</f>
-        <v>217.15521296965107</v>
+        <f t="shared" si="31"/>
+        <v>-17.075994688709628</v>
       </c>
       <c r="AC19" s="5">
-        <f>AB19+AB13</f>
-        <v>330.98398583748212</v>
+        <f t="shared" si="31"/>
+        <v>44.034335437750187</v>
       </c>
       <c r="AD19" s="5">
-        <f>AC19+AC13</f>
-        <v>450.39384260280758</v>
+        <f t="shared" si="31"/>
+        <v>108.90947234125768</v>
       </c>
       <c r="AE19" s="5">
-        <f>AD19+AD13</f>
-        <v>564.56175357557254</v>
+        <f t="shared" si="31"/>
+        <v>166.44735955285199</v>
       </c>
       <c r="AF19" s="5">
-        <f>AE19+AE13</f>
-        <v>672.7462657236739</v>
+        <f t="shared" si="31"/>
+        <v>215.83909230041425</v>
       </c>
       <c r="AG19" s="5">
-        <f>AF19+AF13</f>
-        <v>774.15304286529363</v>
+        <f t="shared" si="31"/>
+        <v>256.22081318368015</v>
       </c>
     </row>
     <row r="20" spans="2:79" s="7" customFormat="1" x14ac:dyDescent="0.25">
@@ -3780,71 +3863,59 @@
       <c r="N21" s="6"/>
       <c r="P21" s="13"/>
       <c r="Q21" s="21">
-        <f>Q11/Q19</f>
+        <f t="shared" ref="Q21:U21" si="32">Q11/Q19</f>
         <v>-8.9935561633674832E-2</v>
       </c>
       <c r="R21" s="21">
-        <f>R11/R19</f>
+        <f t="shared" si="32"/>
         <v>-0.10915776169137079</v>
       </c>
       <c r="S21" s="21">
-        <f>S11/S19</f>
+        <f t="shared" si="32"/>
         <v>-9.2235294117647068E-2</v>
       </c>
       <c r="T21" s="21">
-        <f>T11/T19</f>
+        <f t="shared" si="32"/>
         <v>-8.0247457179340412E-2</v>
       </c>
       <c r="U21" s="21">
-        <f>U11/U19</f>
+        <f t="shared" si="32"/>
         <v>-0.10977560414269276</v>
       </c>
       <c r="V21" s="21">
-        <f>V11/V19</f>
         <v>-0.10500000000000001</v>
       </c>
       <c r="W21" s="21">
-        <f>W11/W19</f>
         <v>-0.10500000000000001</v>
       </c>
       <c r="X21" s="21">
-        <f>X11/X19</f>
         <v>-0.105</v>
       </c>
       <c r="Y21" s="21">
-        <f>Y11/Y19</f>
         <v>-0.105</v>
       </c>
       <c r="Z21" s="21">
-        <f>Z11/Z19</f>
         <v>-1.5000000000000001E-2</v>
       </c>
       <c r="AA21" s="21">
-        <f>AA11/AA19</f>
         <v>-1.5000000000000001E-2</v>
       </c>
       <c r="AB21" s="21">
-        <f>AB11/AB19</f>
         <v>-1.4999999999999999E-2</v>
       </c>
       <c r="AC21" s="21">
-        <f>AC11/AC19</f>
         <v>-0.01</v>
       </c>
       <c r="AD21" s="21">
-        <f>AD11/AD19</f>
         <v>-0.01</v>
       </c>
       <c r="AE21" s="21">
-        <f>AE11/AE19</f>
         <v>-0.01</v>
       </c>
       <c r="AF21" s="21">
-        <f>AF11/AF19</f>
         <v>-0.01</v>
       </c>
       <c r="AG21" s="21">
-        <f>AG11/AG19</f>
         <v>-0.01</v>
       </c>
       <c r="AH21" s="1"/>
@@ -3936,7 +4007,7 @@
         <v>42</v>
       </c>
       <c r="AK22" s="9">
-        <v>0.08</v>
+        <v>7.0000000000000007E-2</v>
       </c>
       <c r="AL22" s="1"/>
       <c r="AM22" s="1"/>
@@ -3994,111 +4065,105 @@
         <v>0.59393756207090109</v>
       </c>
       <c r="E23" s="10">
-        <f t="shared" ref="E23:K23" si="15">E5/E3</f>
+        <f t="shared" ref="E23:K23" si="33">E5/E3</f>
         <v>0.58863675140760963</v>
       </c>
       <c r="F23" s="10">
-        <f t="shared" si="15"/>
+        <f t="shared" si="33"/>
         <v>0.56711675933280381</v>
       </c>
       <c r="G23" s="10">
-        <f t="shared" si="15"/>
+        <f t="shared" si="33"/>
         <v>0.68040278853601865</v>
       </c>
       <c r="H23" s="10">
-        <f t="shared" si="15"/>
+        <f t="shared" si="33"/>
         <v>0.68674244803114992</v>
       </c>
       <c r="I23" s="10">
-        <f t="shared" si="15"/>
+        <f t="shared" si="33"/>
         <v>0.68892110986620969</v>
       </c>
       <c r="J23" s="10">
-        <f t="shared" si="15"/>
+        <f t="shared" si="33"/>
         <v>0.63878746124698582</v>
       </c>
       <c r="K23" s="10">
-        <f t="shared" si="15"/>
+        <f t="shared" si="33"/>
         <v>0.69694847487409994</v>
       </c>
-      <c r="L23" s="10"/>
-      <c r="M23" s="10"/>
+      <c r="L23" s="10">
+        <f>L5/L3</f>
+        <v>0.70144692528377195</v>
+      </c>
+      <c r="M23" s="10">
+        <f>M5/M3</f>
+        <v>0.69920106524633818</v>
+      </c>
       <c r="N23" s="10"/>
       <c r="P23" s="14"/>
       <c r="Q23" s="10">
-        <f t="shared" ref="Q23" si="16">Q5/Q3</f>
+        <f t="shared" ref="Q23" si="34">Q5/Q3</f>
         <v>0.71565678269588884</v>
       </c>
       <c r="R23" s="10">
-        <f t="shared" ref="R23:T23" si="17">R5/R3</f>
+        <f t="shared" ref="R23:T23" si="35">R5/R3</f>
         <v>0.70437491151068943</v>
       </c>
       <c r="S23" s="10">
-        <f t="shared" si="17"/>
+        <f t="shared" si="35"/>
         <v>0.61990452770143212</v>
       </c>
       <c r="T23" s="10">
-        <f t="shared" si="17"/>
+        <f t="shared" si="35"/>
         <v>0.57552053430195083</v>
       </c>
       <c r="U23" s="10">
-        <f t="shared" ref="U23:V23" si="18">U5/U3</f>
+        <f t="shared" ref="U23" si="36">U5/U3</f>
         <v>0.67401445634900292</v>
       </c>
       <c r="V23" s="10">
-        <f t="shared" si="18"/>
-        <v>0.66</v>
+        <v>0.7</v>
       </c>
       <c r="W23" s="10">
-        <f t="shared" ref="W23:AG23" si="19">W5/W3</f>
-        <v>0.66</v>
+        <v>0.7</v>
       </c>
       <c r="X23" s="10">
-        <f t="shared" si="19"/>
-        <v>0.66</v>
+        <v>0.7</v>
       </c>
       <c r="Y23" s="10">
-        <f t="shared" si="19"/>
-        <v>0.66</v>
+        <v>0.7</v>
       </c>
       <c r="Z23" s="10">
-        <f t="shared" si="19"/>
-        <v>0.65999999999999992</v>
+        <v>0.7</v>
       </c>
       <c r="AA23" s="10">
-        <f t="shared" si="19"/>
-        <v>0.66</v>
+        <v>0.7</v>
       </c>
       <c r="AB23" s="10">
-        <f t="shared" si="19"/>
-        <v>0.66</v>
+        <v>0.7</v>
       </c>
       <c r="AC23" s="10">
-        <f t="shared" si="19"/>
-        <v>0.66</v>
+        <v>0.7</v>
       </c>
       <c r="AD23" s="10">
-        <f t="shared" si="19"/>
-        <v>0.66000000000000014</v>
+        <v>0.7</v>
       </c>
       <c r="AE23" s="10">
-        <f t="shared" si="19"/>
-        <v>0.66</v>
+        <v>0.7</v>
       </c>
       <c r="AF23" s="10">
-        <f t="shared" si="19"/>
-        <v>0.66</v>
+        <v>0.7</v>
       </c>
       <c r="AG23" s="10">
-        <f t="shared" si="19"/>
-        <v>0.66</v>
+        <v>0.7</v>
       </c>
       <c r="AJ23" s="9" t="s">
         <v>41</v>
       </c>
       <c r="AK23" s="23">
-        <f>NPV(AK22,AH13:HH13)</f>
-        <v>884.42815622737601</v>
+        <f>NPV(AK22,W13:HH13)</f>
+        <v>383.97913711009818</v>
       </c>
     </row>
     <row r="24" spans="2:79" s="9" customFormat="1" x14ac:dyDescent="0.25">
@@ -4106,112 +4171,125 @@
         <v>33</v>
       </c>
       <c r="C24" s="10">
-        <f t="shared" ref="C24" si="20">C9/C3</f>
+        <f t="shared" ref="C24" si="37">C9/C3</f>
         <v>-0.98639096835185613</v>
       </c>
       <c r="D24" s="10">
-        <f t="shared" ref="D24:K24" si="21">D9/D3</f>
+        <f t="shared" ref="D24:K24" si="38">D9/D3</f>
         <v>-0.23518934323589108</v>
       </c>
       <c r="E24" s="10">
-        <f t="shared" si="21"/>
+        <f t="shared" si="38"/>
         <v>-0.20394130694420753</v>
       </c>
       <c r="F24" s="10">
-        <f t="shared" si="21"/>
+        <f t="shared" si="38"/>
         <v>-0.2262430500397139</v>
       </c>
       <c r="G24" s="10">
-        <f t="shared" si="21"/>
+        <f t="shared" si="38"/>
         <v>6.7699457784663131E-2</v>
       </c>
       <c r="H24" s="10">
-        <f t="shared" si="21"/>
+        <f t="shared" si="38"/>
         <v>0.14758525403504366</v>
       </c>
       <c r="I24" s="10">
-        <f t="shared" si="21"/>
+        <f t="shared" si="38"/>
         <v>0.12522243458775439</v>
       </c>
       <c r="J24" s="10">
-        <f t="shared" si="21"/>
+        <f t="shared" si="38"/>
         <v>5.1808473992421701E-2</v>
       </c>
       <c r="K24" s="10">
-        <f t="shared" si="21"/>
+        <f t="shared" si="38"/>
         <v>0.15196505994180903</v>
       </c>
-      <c r="L24" s="10"/>
-      <c r="M24" s="10"/>
+      <c r="L24" s="10">
+        <f t="shared" ref="L24" si="39">L9/L3</f>
+        <v>0.17580765872520887</v>
+      </c>
+      <c r="M24" s="10">
+        <f>M9/M3</f>
+        <v>0.1254993342210384</v>
+      </c>
       <c r="N24" s="10"/>
       <c r="P24" s="14"/>
       <c r="Q24" s="10">
-        <f t="shared" ref="P24:T24" si="22">Q9/Q3</f>
+        <f t="shared" ref="Q24:T24" si="40">Q9/Q3</f>
         <v>0.1398080504225756</v>
       </c>
       <c r="R24" s="10">
-        <f t="shared" si="22"/>
+        <f t="shared" si="40"/>
         <v>0.12388503468780963</v>
       </c>
       <c r="S24" s="10">
-        <f t="shared" si="22"/>
+        <f t="shared" si="40"/>
         <v>7.021553594676691E-2</v>
       </c>
       <c r="T24" s="10">
-        <f t="shared" si="22"/>
+        <f t="shared" si="40"/>
         <v>-0.38410686039018099</v>
       </c>
       <c r="U24" s="10">
-        <f t="shared" ref="U24:V24" si="23">U9/U3</f>
+        <f t="shared" ref="U24:AG24" si="41">U9/U3</f>
         <v>0.10040840040327403</v>
       </c>
       <c r="V24" s="10">
-        <f t="shared" si="23"/>
-        <v>9.8998147311054344E-2</v>
+        <f t="shared" si="41"/>
+        <v>0.13899814731105431</v>
       </c>
       <c r="W24" s="10">
-        <f t="shared" ref="W24:AG24" si="24">W9/W3</f>
-        <v>0.1094841632491655</v>
+        <f t="shared" si="41"/>
+        <v>5.9726146387616377E-2</v>
       </c>
       <c r="X24" s="10">
-        <f t="shared" si="24"/>
-        <v>0.11977417888936809</v>
+        <f t="shared" si="41"/>
+        <v>8.8829503369997495E-2</v>
       </c>
       <c r="Y24" s="10">
-        <f t="shared" si="24"/>
-        <v>0.12987185778863222</v>
+        <f t="shared" si="41"/>
+        <v>8.8829503369997495E-2</v>
       </c>
       <c r="Z24" s="10">
-        <f t="shared" si="24"/>
-        <v>0.13978079502622781</v>
+        <f t="shared" si="41"/>
+        <v>0.10025325097055825</v>
       </c>
       <c r="AA24" s="10">
-        <f t="shared" si="24"/>
-        <v>0.13978079502622789</v>
+        <f t="shared" si="41"/>
+        <v>0.11146347057858526</v>
       </c>
       <c r="AB24" s="10">
-        <f t="shared" si="24"/>
-        <v>0.13978079502622787</v>
+        <f t="shared" si="41"/>
+        <v>0.11146347057858508</v>
       </c>
       <c r="AC24" s="10">
-        <f t="shared" si="24"/>
-        <v>0.13978079502622789</v>
+        <f t="shared" si="41"/>
+        <v>0.11146347057858509</v>
       </c>
       <c r="AD24" s="10">
-        <f t="shared" si="24"/>
-        <v>0.12967945124032942</v>
+        <f t="shared" si="41"/>
+        <v>0.10003557680341207</v>
       </c>
       <c r="AE24" s="10">
-        <f t="shared" si="24"/>
-        <v>0.11938196485664651</v>
+        <f t="shared" si="41"/>
+        <v>8.8385782178235534E-2</v>
       </c>
       <c r="AF24" s="10">
-        <f t="shared" si="24"/>
-        <v>0.10888452728104736</v>
+        <f t="shared" si="41"/>
+        <v>7.6509777948686741E-2</v>
       </c>
       <c r="AG24" s="10">
-        <f t="shared" si="24"/>
-        <v>8.7058171925841324E-2</v>
+        <f t="shared" si="41"/>
+        <v>5.1817095887248657E-2</v>
+      </c>
+      <c r="AJ24" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="AK24" s="23">
+        <f>AK23/M14</f>
+        <v>27.501728771672983</v>
       </c>
     </row>
     <row r="25" spans="2:79" s="9" customFormat="1" x14ac:dyDescent="0.25">
@@ -4219,55 +4297,61 @@
         <v>29</v>
       </c>
       <c r="C25" s="24">
-        <f t="shared" ref="C25:F25" si="25">C12/C3</f>
+        <f t="shared" ref="C25:F25" si="42">C12/C3</f>
         <v>-0.26492541415207382</v>
       </c>
       <c r="D25" s="24">
-        <f t="shared" si="25"/>
+        <f t="shared" si="42"/>
         <v>-7.5564575327086672E-2</v>
       </c>
       <c r="E25" s="24">
-        <f t="shared" si="25"/>
+        <f t="shared" si="42"/>
         <v>-6.2386964681794915E-2</v>
       </c>
       <c r="F25" s="24">
-        <f t="shared" si="25"/>
+        <f t="shared" si="42"/>
         <v>-7.7037331215250193E-2</v>
       </c>
       <c r="G25" s="24">
-        <f>G12/G3</f>
+        <f t="shared" ref="G25:M25" si="43">G12/G3</f>
         <v>1.0782339271882262E-2</v>
       </c>
       <c r="H25" s="24">
-        <f>H12/H3</f>
+        <f t="shared" si="43"/>
         <v>2.7909313571563149E-2</v>
       </c>
       <c r="I25" s="24">
-        <f>I12/I3</f>
+        <f t="shared" si="43"/>
         <v>1.7069795030646543E-2</v>
       </c>
       <c r="J25" s="24">
-        <f>J12/J3</f>
+        <f t="shared" si="43"/>
         <v>-2.8384429900103337E-3</v>
       </c>
       <c r="K25" s="24">
-        <f>K12/K3</f>
+        <f t="shared" si="43"/>
         <v>3.1896809682368896E-2</v>
       </c>
-      <c r="L25" s="10"/>
-      <c r="M25" s="10"/>
+      <c r="L25" s="24">
+        <f t="shared" si="43"/>
+        <v>3.687164774853436E-2</v>
+      </c>
+      <c r="M25" s="24">
+        <f t="shared" si="43"/>
+        <v>2.9893475366178434E-2</v>
+      </c>
       <c r="N25" s="10"/>
       <c r="P25" s="14"/>
       <c r="Q25" s="21">
-        <f t="shared" ref="Q25:S25" si="26">Q12/Q3</f>
+        <f t="shared" ref="Q25:S25" si="44">Q12/Q3</f>
         <v>-7.7352814782982379E-3</v>
       </c>
       <c r="R25" s="21">
-        <f t="shared" si="26"/>
+        <f t="shared" si="44"/>
         <v>1.6423616027183917E-2</v>
       </c>
       <c r="S25" s="21">
-        <f t="shared" si="26"/>
+        <f t="shared" si="44"/>
         <v>-4.3396499349052514E-3</v>
       </c>
       <c r="T25" s="21">
@@ -4279,52 +4363,40 @@
         <v>1.3694229421916919E-2</v>
       </c>
       <c r="V25" s="21">
-        <f>V12/V3</f>
-        <v>1.7999999999999999E-2</v>
+        <v>3.3000000000000002E-2</v>
       </c>
       <c r="W25" s="21">
-        <f t="shared" ref="W25:AG25" si="27">W12/W3</f>
-        <v>1.7999999999999999E-2</v>
+        <v>3.4000000000000002E-2</v>
       </c>
       <c r="X25" s="21">
-        <f t="shared" si="27"/>
-        <v>1.7999999999999999E-2</v>
+        <v>3.5000000000000003E-2</v>
       </c>
       <c r="Y25" s="21">
-        <f t="shared" si="27"/>
-        <v>1.7999999999999999E-2</v>
+        <v>3.5000000000000003E-2</v>
       </c>
       <c r="Z25" s="21">
-        <f t="shared" si="27"/>
-        <v>1.7999999999999999E-2</v>
+        <v>3.5000000000000003E-2</v>
       </c>
       <c r="AA25" s="21">
-        <f t="shared" si="27"/>
-        <v>1.7999999999999999E-2</v>
+        <v>3.5000000000000003E-2</v>
       </c>
       <c r="AB25" s="21">
-        <f t="shared" si="27"/>
-        <v>1.7999999999999999E-2</v>
+        <v>3.5000000000000003E-2</v>
       </c>
       <c r="AC25" s="21">
-        <f t="shared" si="27"/>
-        <v>1.7999999999999999E-2</v>
+        <v>3.5000000000000003E-2</v>
       </c>
       <c r="AD25" s="21">
-        <f t="shared" si="27"/>
-        <v>1.7999999999999999E-2</v>
+        <v>3.5000000000000003E-2</v>
       </c>
       <c r="AE25" s="21">
-        <f t="shared" si="27"/>
-        <v>1.7999999999999999E-2</v>
+        <v>3.5000000000000003E-2</v>
       </c>
       <c r="AF25" s="21">
-        <f t="shared" si="27"/>
-        <v>1.7999999999999999E-2</v>
+        <v>3.5000000000000003E-2</v>
       </c>
       <c r="AG25" s="21">
-        <f t="shared" si="27"/>
-        <v>1.7999999999999999E-2</v>
+        <v>3.5000000000000003E-2</v>
       </c>
       <c r="AJ25" s="10"/>
       <c r="AK25" s="10"/>
@@ -4376,40 +4448,48 @@
         <v>34</v>
       </c>
       <c r="C26" s="10">
-        <f t="shared" ref="C26" si="28">C3/C6</f>
+        <f t="shared" ref="C26" si="45">C3/C6</f>
         <v>1.034914675767918</v>
       </c>
       <c r="D26" s="10">
-        <f t="shared" ref="D26:J26" si="29">D3/D6</f>
+        <f t="shared" ref="D26:I26" si="46">D3/D6</f>
         <v>1.1922265122265121</v>
       </c>
       <c r="E26" s="10">
-        <f t="shared" si="29"/>
+        <f t="shared" si="46"/>
         <v>1.2741304347826088</v>
       </c>
       <c r="F26" s="10">
-        <f t="shared" si="29"/>
+        <f t="shared" si="46"/>
         <v>1.4707943925233646</v>
       </c>
       <c r="G26" s="10">
-        <f t="shared" si="29"/>
+        <f t="shared" si="46"/>
         <v>1.6321112515802783</v>
       </c>
       <c r="H26" s="10">
-        <f t="shared" si="29"/>
+        <f t="shared" si="46"/>
         <v>1.8547466511357018</v>
       </c>
       <c r="I26" s="10">
-        <f t="shared" si="29"/>
+        <f t="shared" si="46"/>
         <v>1.7739974278031099</v>
       </c>
       <c r="J26" s="10">
-        <f t="shared" si="29"/>
+        <f>J3/J6</f>
         <v>1.7036384976525822</v>
       </c>
       <c r="K26" s="10">
         <f>K3/K6</f>
         <v>1.8349182242990654</v>
+      </c>
+      <c r="L26" s="10">
+        <f>L3/L6</f>
+        <v>1.9024453910133956</v>
+      </c>
+      <c r="M26" s="10">
+        <f>M3/M6</f>
+        <v>1.7697655237421936</v>
       </c>
       <c r="P26" s="20"/>
       <c r="Q26" s="10">
@@ -4417,11 +4497,11 @@
         <v>1.7365671641791045</v>
       </c>
       <c r="R26" s="10">
-        <f t="shared" ref="R26:S26" si="30">R3/R6</f>
+        <f t="shared" ref="R26:S26" si="47">R3/R6</f>
         <v>1.7226829268292683</v>
       </c>
       <c r="S26" s="10">
-        <f t="shared" si="30"/>
+        <f t="shared" si="47"/>
         <v>1.8192105263157894</v>
       </c>
       <c r="T26" s="10">
@@ -4437,48 +4517,48 @@
         <v>1.7825253075491396</v>
       </c>
       <c r="W26" s="10">
-        <f t="shared" ref="W26:AG26" si="31">W3/W6</f>
-        <v>1.8164781705500757</v>
+        <f t="shared" ref="W26:AG26" si="48">W3/W6</f>
+        <v>1.5618316980430558</v>
       </c>
       <c r="X26" s="10">
-        <f t="shared" si="31"/>
-        <v>1.8510777547510295</v>
+        <f t="shared" si="48"/>
+        <v>1.6362046360451061</v>
       </c>
       <c r="Y26" s="10">
-        <f t="shared" si="31"/>
-        <v>1.8863363786510492</v>
+        <f t="shared" si="48"/>
+        <v>1.6362046360451061</v>
       </c>
       <c r="Z26" s="10">
-        <f t="shared" si="31"/>
-        <v>1.9222665953872597</v>
+        <f t="shared" si="48"/>
+        <v>1.6673704386364414</v>
       </c>
       <c r="AA26" s="10">
-        <f t="shared" si="31"/>
-        <v>1.9222665953872597</v>
+        <f t="shared" si="48"/>
+        <v>1.6991298755628499</v>
       </c>
       <c r="AB26" s="10">
-        <f t="shared" si="31"/>
-        <v>1.9222665953872597</v>
+        <f t="shared" si="48"/>
+        <v>1.6991298755628497</v>
       </c>
       <c r="AC26" s="10">
-        <f t="shared" si="31"/>
-        <v>1.9222665953872597</v>
+        <f t="shared" si="48"/>
+        <v>1.6991298755628497</v>
       </c>
       <c r="AD26" s="10">
-        <f t="shared" si="31"/>
-        <v>1.8856519935703595</v>
+        <f t="shared" si="48"/>
+        <v>1.6667654969807002</v>
       </c>
       <c r="AE26" s="10">
-        <f t="shared" si="31"/>
-        <v>1.849734812740448</v>
+        <f t="shared" si="48"/>
+        <v>1.6350175827524964</v>
       </c>
       <c r="AF26" s="10">
-        <f t="shared" si="31"/>
-        <v>1.814501768688249</v>
+        <f t="shared" si="48"/>
+        <v>1.6038743907000679</v>
       </c>
       <c r="AG26" s="10">
-        <f t="shared" si="31"/>
-        <v>1.7453778917858396</v>
+        <f t="shared" si="48"/>
+        <v>1.5427744139114938</v>
       </c>
     </row>
     <row r="27" spans="2:79" x14ac:dyDescent="0.25">
@@ -4495,27 +4575,33 @@
       <c r="E28" s="10"/>
       <c r="F28" s="10"/>
       <c r="G28" s="10">
-        <f t="shared" ref="G28:J28" si="32">G3/C3-1</f>
+        <f t="shared" ref="G28:J28" si="49">G3/C3-1</f>
         <v>0.41916477041629574</v>
       </c>
       <c r="H28" s="10">
-        <f t="shared" si="32"/>
+        <f t="shared" si="49"/>
         <v>0.71887818990457264</v>
       </c>
       <c r="I28" s="10">
-        <f t="shared" si="32"/>
+        <f t="shared" si="49"/>
         <v>0.29440368537792172</v>
       </c>
       <c r="J28" s="10">
-        <f t="shared" si="32"/>
+        <f t="shared" si="49"/>
         <v>0.1528991262907069</v>
       </c>
       <c r="K28" s="10">
         <f>K3/G3-1</f>
         <v>0.21664601084430668</v>
       </c>
-      <c r="L28" s="10"/>
-      <c r="M28" s="10"/>
+      <c r="L28" s="10">
+        <f>L3/H3-1</f>
+        <v>6.9710481693148196E-3</v>
+      </c>
+      <c r="M28" s="10">
+        <f>M3/I3-1</f>
+        <v>-1.0083701311540239E-2</v>
+      </c>
       <c r="N28" s="10"/>
       <c r="P28" s="14"/>
       <c r="R28" s="10">
@@ -4523,11 +4609,11 @@
         <v>1.1746168170749138E-2</v>
       </c>
       <c r="S28" s="10">
-        <f t="shared" ref="R28:T28" si="33">S3/R3-1</f>
+        <f t="shared" ref="S28:T28" si="50">S3/R3-1</f>
         <v>-2.123743451791027E-2</v>
       </c>
       <c r="T28" s="10">
-        <f t="shared" si="33"/>
+        <f t="shared" si="50"/>
         <v>-0.38272096050918547</v>
       </c>
       <c r="U28" s="10">
@@ -4539,48 +4625,37 @@
         <v>7.3590676851045034E-2</v>
       </c>
       <c r="W28" s="10">
-        <f t="shared" ref="W28:AG28" si="34">W3/V3-1</f>
-        <v>7.0000000000000062E-2</v>
+        <v>-0.08</v>
       </c>
       <c r="X28" s="10">
-        <f t="shared" si="34"/>
-        <v>7.0000000000000062E-2</v>
+        <v>0.1</v>
       </c>
       <c r="Y28" s="10">
-        <f t="shared" si="34"/>
-        <v>7.0000000000000062E-2</v>
+        <v>0.05</v>
       </c>
       <c r="Z28" s="10">
-        <f t="shared" si="34"/>
-        <v>7.0000000000000062E-2</v>
+        <v>7.0000000000000007E-2</v>
       </c>
       <c r="AA28" s="10">
-        <f t="shared" si="34"/>
-        <v>5.0000000000000044E-2</v>
+        <v>7.0000000000000007E-2</v>
       </c>
       <c r="AB28" s="10">
-        <f t="shared" si="34"/>
-        <v>5.0000000000000044E-2</v>
+        <v>0.05</v>
       </c>
       <c r="AC28" s="10">
-        <f t="shared" si="34"/>
-        <v>5.0000000000000044E-2</v>
+        <v>0.05</v>
       </c>
       <c r="AD28" s="10">
-        <f t="shared" si="34"/>
-        <v>3.0000000000000027E-2</v>
+        <v>0.03</v>
       </c>
       <c r="AE28" s="10">
-        <f t="shared" si="34"/>
-        <v>3.0000000000000027E-2</v>
+        <v>0.03</v>
       </c>
       <c r="AF28" s="10">
-        <f t="shared" si="34"/>
-        <v>3.0000000000000027E-2</v>
+        <v>0.03</v>
       </c>
       <c r="AG28" s="10">
-        <f t="shared" si="34"/>
-        <v>1.0000000000000009E-2</v>
+        <v>0.01</v>
       </c>
     </row>
     <row r="29" spans="2:79" s="9" customFormat="1" x14ac:dyDescent="0.25">
@@ -4598,10 +4673,59 @@
       <c r="K29" s="10" t="s">
         <v>36</v>
       </c>
-      <c r="L29" s="10"/>
-      <c r="M29" s="10"/>
+      <c r="L29" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="M29" s="10">
+        <f>M13/I13-1</f>
+        <v>-0.20661745085831285</v>
+      </c>
       <c r="N29" s="10"/>
       <c r="P29" s="14"/>
+      <c r="W29" s="9">
+        <f>W13/V13-1</f>
+        <v>-1.0343935836435614</v>
+      </c>
+      <c r="X29" s="9">
+        <f t="shared" ref="X29:AG29" si="51">X13/W13-1</f>
+        <v>-12.291321232831914</v>
+      </c>
+      <c r="Y29" s="9">
+        <f t="shared" si="51"/>
+        <v>0.20206526904841815</v>
+      </c>
+      <c r="Z29" s="9">
+        <f t="shared" si="51"/>
+        <v>1.1150941761250941</v>
+      </c>
+      <c r="AA29" s="9">
+        <f t="shared" si="51"/>
+        <v>0.27894835322539979</v>
+      </c>
+      <c r="AB29" s="9">
+        <f t="shared" si="51"/>
+        <v>6.597339786140477E-2</v>
+      </c>
+      <c r="AC29" s="9">
+        <f t="shared" si="51"/>
+        <v>6.1606716397324401E-2</v>
+      </c>
+      <c r="AD29" s="9">
+        <f t="shared" si="51"/>
+        <v>-0.11309802248011147</v>
+      </c>
+      <c r="AE29" s="9">
+        <f t="shared" si="51"/>
+        <v>-0.14157896403242498</v>
+      </c>
+      <c r="AF29" s="9">
+        <f t="shared" si="51"/>
+        <v>-0.18241943262743809</v>
+      </c>
+      <c r="AG29" s="9">
+        <f t="shared" si="51"/>
+        <v>-0.54923409987846694</v>
+      </c>
     </row>
     <row r="30" spans="2:79" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C30" s="10"/>
@@ -4619,6 +4743,9 @@
       <c r="P30" s="14"/>
     </row>
     <row r="31" spans="2:79" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B31" s="9" t="s">
+        <v>46</v>
+      </c>
       <c r="C31" s="10"/>
       <c r="D31" s="10"/>
       <c r="E31" s="10"/>
@@ -4626,6 +4753,22 @@
       <c r="G31" s="10"/>
       <c r="H31" s="10"/>
       <c r="P31" s="14"/>
+      <c r="R31" s="9">
+        <f t="shared" ref="R31:T31" si="52">R6/Q6-1</f>
+        <v>1.990049751243772E-2</v>
+      </c>
+      <c r="S31" s="9">
+        <f t="shared" si="52"/>
+        <v>-7.3170731707317027E-2</v>
+      </c>
+      <c r="T31" s="9">
+        <f t="shared" si="52"/>
+        <v>-9.6842105263157729E-2</v>
+      </c>
+      <c r="U31" s="9">
+        <f>U6/T6-1</f>
+        <v>-2.1911421911422035E-2</v>
+      </c>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>

</xml_diff>